<commit_message>
step 3 - calculate {     - GRP1, GRP 2 }
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B6E58B-4C36-47DF-AA77-F744231DAB53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5530DB9B-5DDD-425F-95B1-1508C15742A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="плотностьНаселения" sheetId="3" r:id="rId3"/>
+    <sheet name="GRP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>CH4</t>
   </si>
@@ -117,6 +120,57 @@
   </si>
   <si>
     <t>V N2 =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V пр см = </t>
+  </si>
+  <si>
+    <t>№ кв</t>
+  </si>
+  <si>
+    <t>этажность</t>
+  </si>
+  <si>
+    <t>площадь</t>
+  </si>
+  <si>
+    <t>коло-во жит.</t>
+  </si>
+  <si>
+    <t>плотность начеоения</t>
+  </si>
+  <si>
+    <t>η =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R опт = </t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>ГРП 1</t>
+  </si>
+  <si>
+    <t>ГРП 2</t>
+  </si>
+  <si>
+    <t>общая численность населения</t>
+  </si>
+  <si>
+    <t>5 эт</t>
+  </si>
+  <si>
+    <t>7 эт</t>
+  </si>
+  <si>
+    <t>8 эт</t>
+  </si>
+  <si>
+    <t>6 эт</t>
+  </si>
+  <si>
+    <t>9 эт</t>
   </si>
 </sst>
 </file>
@@ -150,15 +204,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -166,11 +232,240 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -179,6 +474,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,9 +1118,1393 @@
         <v>8.3802227800000022</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <f>B26+B28+B32+B30</f>
+        <v>11.60033051245202</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879CB410-EB40-41A7-8023-5EC270239CE9}">
+  <dimension ref="A1:U29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="6" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" customWidth="1"/>
+    <col min="20" max="20" width="4.85546875" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="D2" s="5">
+        <f>VLOOKUP(B2,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>230</v>
+      </c>
+      <c r="E2" s="5">
+        <f>ROUNDUP(C2*D2,0)</f>
+        <v>897</v>
+      </c>
+      <c r="H2" s="30">
+        <f>B2</f>
+        <v>5</v>
+      </c>
+      <c r="I2" s="4">
+        <f>E2</f>
+        <v>897</v>
+      </c>
+      <c r="J2" s="16">
+        <v>5</v>
+      </c>
+      <c r="K2" s="16">
+        <v>6</v>
+      </c>
+      <c r="L2" s="16">
+        <v>7</v>
+      </c>
+      <c r="M2" s="16">
+        <v>8</v>
+      </c>
+      <c r="N2" s="17">
+        <v>9</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="16">
+        <v>5</v>
+      </c>
+      <c r="R2" s="16">
+        <v>6</v>
+      </c>
+      <c r="S2" s="16">
+        <v>7</v>
+      </c>
+      <c r="T2" s="16">
+        <v>8</v>
+      </c>
+      <c r="U2" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="D3" s="5">
+        <f>VLOOKUP(B3,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E27" si="0">ROUNDUP(C3*D3,0)</f>
+        <v>1670</v>
+      </c>
+      <c r="H3" s="30">
+        <f t="shared" ref="H3:H6" si="1">B3</f>
+        <v>8</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I28" si="2">E3</f>
+        <v>1670</v>
+      </c>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="19"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <f>VLOOKUP(B4,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>420</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>1899</v>
+      </c>
+      <c r="H4" s="30">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="2"/>
+        <v>1899</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="19"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10.59</v>
+      </c>
+      <c r="D5" s="5">
+        <f>VLOOKUP(B5,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>3707</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>3707</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="19"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>11.98</v>
+      </c>
+      <c r="D6" s="5">
+        <f>VLOOKUP(B6,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>420</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>5032</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="2"/>
+        <v>5032</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>16.64</v>
+      </c>
+      <c r="D7" s="5">
+        <f>VLOOKUP(B7,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>5824</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="29">
+        <f>B7</f>
+        <v>7</v>
+      </c>
+      <c r="P7" s="4">
+        <f>E7</f>
+        <v>5824</v>
+      </c>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="19"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7.98</v>
+      </c>
+      <c r="D8" s="5">
+        <f>VLOOKUP(B8,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>2793</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="29">
+        <f t="shared" ref="O8:O12" si="3">B8</f>
+        <v>8</v>
+      </c>
+      <c r="P8" s="4">
+        <f>E8</f>
+        <v>2793</v>
+      </c>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="19"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>9.93</v>
+      </c>
+      <c r="D9" s="5">
+        <f>VLOOKUP(B9,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>3476</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="29">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P9" s="4">
+        <f>E9</f>
+        <v>3476</v>
+      </c>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="19"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5.86</v>
+      </c>
+      <c r="D10" s="5">
+        <f>VLOOKUP(B10,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>230</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>1348</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="29">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="4">
+        <f>E10</f>
+        <v>1348</v>
+      </c>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="19"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4">
+        <v>12.99</v>
+      </c>
+      <c r="D11" s="5">
+        <f>VLOOKUP(B11,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>4547</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="29">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P11" s="4">
+        <f>E11</f>
+        <v>4547</v>
+      </c>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="19"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5.85</v>
+      </c>
+      <c r="D12" s="5">
+        <f>VLOOKUP(B12,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="29">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="P12" s="4">
+        <f>E12</f>
+        <v>2048</v>
+      </c>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="19"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.08</v>
+      </c>
+      <c r="D13" s="5">
+        <f>VLOOKUP(B13,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>3178</v>
+      </c>
+      <c r="H13" s="30">
+        <f>B13</f>
+        <v>6</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
+        <v>3178</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="19"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>7.85</v>
+      </c>
+      <c r="D14" s="5">
+        <f>VLOOKUP(B14,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>230</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>1806</v>
+      </c>
+      <c r="H14" s="30">
+        <f t="shared" ref="H14:H20" si="4">B14</f>
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="2"/>
+        <v>1806</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="19"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4.41</v>
+      </c>
+      <c r="D15" s="5">
+        <f>VLOOKUP(B15,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>420</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>1853</v>
+      </c>
+      <c r="H15" s="30">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="2"/>
+        <v>1853</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="19"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3.02</v>
+      </c>
+      <c r="D16" s="5">
+        <f>VLOOKUP(B16,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>1057</v>
+      </c>
+      <c r="H16" s="30">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="2"/>
+        <v>1057</v>
+      </c>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="19"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="D17" s="5">
+        <f>VLOOKUP(B17,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>1757</v>
+      </c>
+      <c r="H17" s="30">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="2"/>
+        <v>1757</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="19"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6.08</v>
+      </c>
+      <c r="D18" s="5">
+        <f>VLOOKUP(B18,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>2128</v>
+      </c>
+      <c r="H18" s="30">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="2"/>
+        <v>2128</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="19"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4">
+        <v>12.87</v>
+      </c>
+      <c r="D19" s="5">
+        <f>VLOOKUP(B19,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>4505</v>
+      </c>
+      <c r="H19" s="30">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="2"/>
+        <v>4505</v>
+      </c>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="19"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="D20" s="5">
+        <f>VLOOKUP(B20,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>230</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>3329</v>
+      </c>
+      <c r="H20" s="30">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="2"/>
+        <v>3329</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="19"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="D21" s="5">
+        <f>VLOOKUP(B21,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>230</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>2156</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="29">
+        <f>B21</f>
+        <v>5</v>
+      </c>
+      <c r="P21" s="4">
+        <f>E21</f>
+        <v>2156</v>
+      </c>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="19"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="D22" s="5">
+        <f>VLOOKUP(B22,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>1645</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="29">
+        <f t="shared" ref="O22:O25" si="5">B22</f>
+        <v>8</v>
+      </c>
+      <c r="P22" s="4">
+        <f>E22</f>
+        <v>1645</v>
+      </c>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="19"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4">
+        <v>4.43</v>
+      </c>
+      <c r="D23" s="5">
+        <f>VLOOKUP(B23,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
+        <v>1551</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="29">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P23" s="4">
+        <f>E23</f>
+        <v>1551</v>
+      </c>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="19"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4">
+        <v>13.76</v>
+      </c>
+      <c r="D24" s="5">
+        <f>VLOOKUP(B24,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>4816</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="29">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P24" s="4">
+        <f>E24</f>
+        <v>4816</v>
+      </c>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="19"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4">
+        <v>12.04</v>
+      </c>
+      <c r="D25" s="5">
+        <f>VLOOKUP(B25,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>420</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>5057</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="29">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P25" s="4">
+        <f>E25</f>
+        <v>5057</v>
+      </c>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="19"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4">
+        <v>12.81</v>
+      </c>
+      <c r="D26" s="5">
+        <f>VLOOKUP(B26,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
+        <v>4484</v>
+      </c>
+      <c r="H26" s="30">
+        <f>B26</f>
+        <v>8</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="2"/>
+        <v>4484</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="D27" s="5">
+        <f>VLOOKUP(B27,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>3486</v>
+      </c>
+      <c r="H27" s="30">
+        <f t="shared" ref="H27:H28" si="6">B27</f>
+        <v>6</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="2"/>
+        <v>3486</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D28" s="5">
+        <f>VLOOKUP(B28,плотностьНаселения!$A$1:$B$10,2,FALSE)</f>
+        <v>350</v>
+      </c>
+      <c r="E28" s="5">
+        <f>ROUNDUP(C28*D28,0)</f>
+        <v>3483</v>
+      </c>
+      <c r="H28" s="31">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="I28" s="20">
+        <f t="shared" si="2"/>
+        <v>3483</v>
+      </c>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f>SUM(C2:C28)</f>
+        <v>234.82999999999996</v>
+      </c>
+      <c r="H29" s="22">
+        <f>COUNT(H2:H28)</f>
+        <v>16</v>
+      </c>
+      <c r="I29" s="23">
+        <f>SUM(I2:I28)</f>
+        <v>44271</v>
+      </c>
+      <c r="J29" s="24">
+        <f>COUNTIF($H$2:$H$28,J2)</f>
+        <v>3</v>
+      </c>
+      <c r="K29" s="24">
+        <f>COUNTIF($H$2:$H$28,K2)</f>
+        <v>3</v>
+      </c>
+      <c r="L29" s="24">
+        <f t="shared" ref="K29:N29" si="7">COUNTIF($H$2:$H$28,L2)</f>
+        <v>3</v>
+      </c>
+      <c r="M29" s="24">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="N29" s="25">
+        <f>COUNTIF($H$2:$H$28,N2)</f>
+        <v>3</v>
+      </c>
+      <c r="O29" s="26">
+        <f>COUNT(O2:O28)</f>
+        <v>11</v>
+      </c>
+      <c r="P29" s="27">
+        <f>SUM(P2:P28)</f>
+        <v>35261</v>
+      </c>
+      <c r="Q29" s="27">
+        <f>COUNTIF($O$2:$O$28,Q2)</f>
+        <v>2</v>
+      </c>
+      <c r="R29" s="27">
+        <f t="shared" ref="R29:U29" si="8">COUNTIF($O$2:$O$28,R2)</f>
+        <v>2</v>
+      </c>
+      <c r="S29" s="27">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="T29" s="27">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="U29" s="28">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="R2:R28"/>
+    <mergeCell ref="S2:S28"/>
+    <mergeCell ref="T2:T28"/>
+    <mergeCell ref="U2:U28"/>
+    <mergeCell ref="J2:J28"/>
+    <mergeCell ref="K2:K28"/>
+    <mergeCell ref="L2:L28"/>
+    <mergeCell ref="M2:M28"/>
+    <mergeCell ref="N2:N28"/>
+    <mergeCell ref="Q2:Q28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7DE714-ADEC-45CA-B127-CCCD2748ADF3}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1D22C8-ECD6-4798-BD57-3882C5B7C7D5}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <f>Sheet2!C29*10000/(2*POWER(B3,2))</f>
+        <v>1.8346093749999997</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1">
+        <f>ROUND(B1,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
step 5 { calculate error state of 'gazoprovod' }
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BF9A92-2336-4898-86A2-2F0BED6BEB8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6687095D-8156-4B72-945E-8D902D9C7693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="расходГазаПотребителями" sheetId="5" r:id="rId5"/>
     <sheet name="РасхСосредоточПотреб" sheetId="6" r:id="rId6"/>
     <sheet name="РасчРасхСосредоточПотр" sheetId="7" r:id="rId7"/>
+    <sheet name="ЧасовыеРасходы" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="150">
   <si>
     <t>CH4</t>
   </si>
@@ -411,6 +412,93 @@
   </si>
   <si>
     <t xml:space="preserve">VРК1 = </t>
+  </si>
+  <si>
+    <t>Наименование потребителя</t>
+  </si>
+  <si>
+    <t>Часовой расход, м3 /ч</t>
+  </si>
+  <si>
+    <t>Часовой расход при аварии, м3 /ч</t>
+  </si>
+  <si>
+    <t>Коэффициент обеспеченности при аварии</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>ГРП-1</t>
+  </si>
+  <si>
+    <t>ГРП-2</t>
+  </si>
+  <si>
+    <t>Больница</t>
+  </si>
+  <si>
+    <t>Хлебозавод</t>
+  </si>
+  <si>
+    <t>БПК</t>
+  </si>
+  <si>
+    <t>РК №1</t>
+  </si>
+  <si>
+    <t>РК №2</t>
+  </si>
+  <si>
+    <t>QвРК2 =</t>
+  </si>
+  <si>
+    <t>QгвРК2 =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VРК2 = </t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>ГРП1</t>
+  </si>
+  <si>
+    <t>ГРП2</t>
+  </si>
+  <si>
+    <t>потери давления</t>
+  </si>
+  <si>
+    <t>Vрэкв =</t>
+  </si>
+  <si>
+    <t>Среднеквадратичный перепад давления</t>
+  </si>
+  <si>
+    <t>А=</t>
+  </si>
+  <si>
+    <t>Рн =</t>
+  </si>
+  <si>
+    <t>Рк =</t>
+  </si>
+  <si>
+    <t>Общая протяженность газопроdjljd</t>
+  </si>
+  <si>
+    <t>∑L =</t>
+  </si>
+  <si>
+    <t>МПа/км</t>
+  </si>
+  <si>
+    <t>Па/м</t>
+  </si>
+  <si>
+    <t>325-426</t>
   </si>
 </sst>
 </file>
@@ -451,7 +539,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,8 +558,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -839,11 +933,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -930,48 +1137,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -979,6 +1144,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -997,22 +1217,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1720,36 +1954,36 @@
         <f>E2</f>
         <v>897</v>
       </c>
-      <c r="J2" s="38">
+      <c r="J2" s="44">
         <v>5</v>
       </c>
-      <c r="K2" s="38">
+      <c r="K2" s="44">
         <v>6</v>
       </c>
-      <c r="L2" s="38">
+      <c r="L2" s="44">
         <v>7</v>
       </c>
-      <c r="M2" s="38">
+      <c r="M2" s="44">
         <v>8</v>
       </c>
-      <c r="N2" s="40">
+      <c r="N2" s="46">
         <v>9</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="38">
+      <c r="Q2" s="44">
         <v>5</v>
       </c>
-      <c r="R2" s="38">
+      <c r="R2" s="44">
         <v>6</v>
       </c>
-      <c r="S2" s="38">
+      <c r="S2" s="44">
         <v>7</v>
       </c>
-      <c r="T2" s="38">
+      <c r="T2" s="44">
         <v>8</v>
       </c>
-      <c r="U2" s="40">
+      <c r="U2" s="46">
         <v>9</v>
       </c>
     </row>
@@ -1779,18 +2013,18 @@
         <f t="shared" ref="I3:I28" si="2">E3</f>
         <v>1670</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="41"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="47"/>
       <c r="O3" s="11"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="41"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="47"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1818,18 +2052,18 @@
         <f t="shared" si="2"/>
         <v>1899</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="41"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="47"/>
       <c r="O4" s="11"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="41"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="47"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -1857,18 +2091,18 @@
         <f t="shared" si="2"/>
         <v>3707</v>
       </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="41"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="47"/>
       <c r="O5" s="11"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="41"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="47"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -1896,18 +2130,18 @@
         <f t="shared" si="2"/>
         <v>5032</v>
       </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="41"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="47"/>
       <c r="O6" s="11"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="41"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="47"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1929,11 +2163,11 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="41"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="25">
         <f>B7</f>
         <v>7</v>
@@ -1942,11 +2176,11 @@
         <f t="shared" ref="P7:P12" si="3">E7</f>
         <v>5824</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="41"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="47"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1968,11 +2202,11 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="41"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="47"/>
       <c r="O8" s="25">
         <f t="shared" ref="O8:O12" si="4">B8</f>
         <v>8</v>
@@ -1981,11 +2215,11 @@
         <f t="shared" si="3"/>
         <v>2793</v>
       </c>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="41"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="47"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -2007,11 +2241,11 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="41"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="47"/>
       <c r="O9" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2020,11 +2254,11 @@
         <f t="shared" si="3"/>
         <v>3476</v>
       </c>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="41"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="45"/>
+      <c r="U9" s="47"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -2046,11 +2280,11 @@
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="41"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="47"/>
       <c r="O10" s="25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -2059,11 +2293,11 @@
         <f t="shared" si="3"/>
         <v>1348</v>
       </c>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="41"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="47"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -2085,11 +2319,11 @@
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="41"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="47"/>
       <c r="O11" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2098,11 +2332,11 @@
         <f t="shared" si="3"/>
         <v>4547</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="41"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="47"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -2124,11 +2358,11 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="41"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="47"/>
       <c r="O12" s="25">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -2137,11 +2371,11 @@
         <f t="shared" si="3"/>
         <v>2048</v>
       </c>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="41"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="47"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -2169,18 +2403,18 @@
         <f t="shared" si="2"/>
         <v>3178</v>
       </c>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="41"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="47"/>
       <c r="O13" s="11"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="41"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="47"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -2208,18 +2442,18 @@
         <f t="shared" si="2"/>
         <v>1806</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="41"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="47"/>
       <c r="O14" s="11"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="41"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="47"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -2247,18 +2481,18 @@
         <f t="shared" si="2"/>
         <v>1853</v>
       </c>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="41"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="47"/>
       <c r="O15" s="11"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="41"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="47"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -2286,18 +2520,18 @@
         <f t="shared" si="2"/>
         <v>1057</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="41"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="11"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="41"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="47"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -2325,18 +2559,18 @@
         <f t="shared" si="2"/>
         <v>1757</v>
       </c>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="41"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="47"/>
       <c r="O17" s="11"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="41"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="47"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -2364,18 +2598,18 @@
         <f t="shared" si="2"/>
         <v>2128</v>
       </c>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="41"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="47"/>
       <c r="O18" s="11"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="39"/>
-      <c r="U18" s="41"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="47"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -2403,18 +2637,18 @@
         <f t="shared" si="2"/>
         <v>4505</v>
       </c>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="41"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="11"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="41"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="47"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2442,18 +2676,18 @@
         <f t="shared" si="2"/>
         <v>3329</v>
       </c>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="41"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="47"/>
       <c r="O20" s="11"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="41"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="47"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -2475,11 +2709,11 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="41"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="47"/>
       <c r="O21" s="25">
         <f>B21</f>
         <v>5</v>
@@ -2488,11 +2722,11 @@
         <f>E21</f>
         <v>2156</v>
       </c>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="41"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="47"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -2514,11 +2748,11 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="41"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="47"/>
       <c r="O22" s="25">
         <f t="shared" ref="O22:O25" si="6">B22</f>
         <v>8</v>
@@ -2527,11 +2761,11 @@
         <f>E22</f>
         <v>1645</v>
       </c>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="41"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="47"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2553,11 +2787,11 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="41"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="47"/>
       <c r="O23" s="25">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -2566,11 +2800,11 @@
         <f>E23</f>
         <v>1551</v>
       </c>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="41"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="47"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -2592,11 +2826,11 @@
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="41"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="47"/>
       <c r="O24" s="25">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -2605,11 +2839,11 @@
         <f>E24</f>
         <v>4816</v>
       </c>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="39"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="41"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="47"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -2631,11 +2865,11 @@
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="41"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="47"/>
       <c r="O25" s="25">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -2644,11 +2878,11 @@
         <f>E25</f>
         <v>5057</v>
       </c>
-      <c r="Q25" s="39"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="41"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="47"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2676,18 +2910,18 @@
         <f t="shared" si="2"/>
         <v>4484</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="41"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="47"/>
       <c r="O26" s="11"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="41"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="47"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -2715,18 +2949,18 @@
         <f t="shared" si="2"/>
         <v>3486</v>
       </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="41"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="47"/>
       <c r="O27" s="11"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="39"/>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="41"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="47"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
@@ -2754,25 +2988,25 @@
         <f t="shared" si="2"/>
         <v>3483</v>
       </c>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="41"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="47"/>
       <c r="O28" s="17"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="39"/>
-      <c r="T28" s="39"/>
-      <c r="U28" s="41"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="47"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29">
         <f>SUM(C2:C28)</f>
         <v>234.82999999999996</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="38">
         <f>SUM(E2:E28)</f>
         <v>79532</v>
       </c>
@@ -3034,7 +3268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33035FD5-04D2-4D7F-99BE-F176EC4254F0}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G6" sqref="G6:J6"/>
     </sheetView>
   </sheetViews>
@@ -3052,50 +3286,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -3130,32 +3364,32 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
@@ -3196,18 +3430,18 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="47"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
@@ -3264,32 +3498,32 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="44"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="47"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
@@ -3329,18 +3563,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="47"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
@@ -3507,8 +3741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD0AAA4-CEDA-4DBB-82AC-0AD67E237AF8}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,13 +3833,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="39" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="3">
         <v>0.8</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="39" t="s">
         <v>68</v>
       </c>
       <c r="H8" s="3">
@@ -3614,7 +3848,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="39" t="s">
         <v>69</v>
       </c>
       <c r="F9">
@@ -3714,7 +3948,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="39" t="s">
         <v>58</v>
       </c>
       <c r="B23">
@@ -3847,7 +4081,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B48">
         <f>$I$42*$I$43*$F$42*F46*POWER(10,-3)</f>
@@ -3856,7 +4090,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B49">
         <f>$F$43*'расчетКол-ваЖит'!P29*POWER(10,-3)</f>
@@ -3865,7 +4099,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B50">
         <f>(3600*SUM(B47:B49))/($F$8*gazProperties!$B$15)</f>
@@ -3883,8 +4117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9ED7318-8A47-492B-BAB1-7E25EB2B5EE2}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,50 +4128,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -3972,27 +4206,27 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>1</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="40" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="30">
@@ -4026,10 +4260,10 @@
       <c r="A6" s="30">
         <v>2</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="40" t="s">
         <v>88</v>
       </c>
       <c r="D6" s="30">
@@ -4063,10 +4297,10 @@
       <c r="A7" s="30">
         <v>3</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="40" t="s">
         <v>89</v>
       </c>
       <c r="D7" s="30">
@@ -4084,7 +4318,7 @@
         <v>521.90407819455618</v>
       </c>
       <c r="H7" s="30">
-        <f t="shared" ref="H6:H7" si="1">E7*G7</f>
+        <f t="shared" ref="H7" si="1">E7*G7</f>
         <v>239553.97189130128</v>
       </c>
       <c r="I7" s="30">
@@ -4100,36 +4334,36 @@
       <c r="A8" s="30">
         <v>4</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="55" t="str">
+      <c r="C8" s="60" t="str">
         <f>РасхСосредоточПотреб!C6&amp;"+"&amp;РасхСосредоточПотреб!C7</f>
         <v>376.27+229.06</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
       <c r="J8" s="30">
         <f>РасхСосредоточПотреб!B6+РасхСосредоточПотреб!B7</f>
         <v>605.33020079843004</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="61" t="s">
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="41" t="s">
         <v>58</v>
       </c>
       <c r="J9" s="28">
@@ -4138,30 +4372,30 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="60"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="65"/>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>1</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="57"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="30">
         <f>РасхСосредоточПотреб!B31</f>
         <v>3484</v>
@@ -4190,13 +4424,13 @@
       <c r="A12" s="30">
         <v>2</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="57"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="30">
         <f>РасхСосредоточПотреб!B32</f>
         <v>13935</v>
@@ -4225,13 +4459,13 @@
       <c r="A13" s="30">
         <v>3</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="57"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="30">
         <f>РасхСосредоточПотреб!B33</f>
         <v>2903</v>
@@ -4257,17 +4491,17 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="63" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="42" t="s">
         <v>58</v>
       </c>
       <c r="J14" s="36">
@@ -4276,24 +4510,24 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <v>1</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="40" t="s">
         <v>101</v>
       </c>
       <c r="C16" s="30" t="s">
@@ -4330,7 +4564,7 @@
       <c r="A17" s="30">
         <v>2</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="40" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="30" t="s">
@@ -4351,7 +4585,7 @@
         <v>1.3880427611557344</v>
       </c>
       <c r="H17" s="30">
-        <f t="shared" ref="H17:H18" si="5">E17*G17</f>
+        <f t="shared" ref="H17" si="5">E17*G17</f>
         <v>287023.92388861848</v>
       </c>
       <c r="I17" s="30">
@@ -4367,10 +4601,10 @@
       <c r="A18" s="30">
         <v>3</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="40" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="30">
@@ -4401,17 +4635,17 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="61" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="41" t="s">
         <v>58</v>
       </c>
       <c r="J19" s="28">
@@ -4420,124 +4654,115 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -4548,6 +4773,350 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC937C0-5E57-457A-81B6-0468CB5DE98C}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="43"/>
+      <c r="K1" s="80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68">
+        <v>2</v>
+      </c>
+      <c r="C2" s="70">
+        <v>3</v>
+      </c>
+      <c r="D2" s="68">
+        <v>4</v>
+      </c>
+      <c r="E2" s="71">
+        <v>5</v>
+      </c>
+      <c r="I2" s="78"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="81"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="5">
+        <f>расходГазаПотребителями!J9</f>
+        <v>1834.8767615750357</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="5">
+        <f>C3*D3</f>
+        <v>1467.9014092600287</v>
+      </c>
+      <c r="I3" s="79">
+        <f>C3</f>
+        <v>1834.8767615750357</v>
+      </c>
+      <c r="K3" s="80"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="4">
+        <f>расходГазаПотребителями!J15</f>
+        <v>1381.5644407283489</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E9" si="0">C4*D4</f>
+        <v>1105.2515525826791</v>
+      </c>
+      <c r="I4" s="82"/>
+      <c r="K4" s="83">
+        <f>C5</f>
+        <v>870.57060066538452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="4">
+        <f>РасчРасхСосредоточПотр!J9</f>
+        <v>870.57060066538452</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>739.98501056557677</v>
+      </c>
+      <c r="I5" s="82"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="4">
+        <f>РасчРасхСосредоточПотр!J14</f>
+        <v>495.78111342960517</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>347.04677940072361</v>
+      </c>
+      <c r="I6" s="82">
+        <f>C6</f>
+        <v>495.78111342960517</v>
+      </c>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="4">
+        <f>РасчРасхСосредоточПотр!J19</f>
+        <v>1643.2228653439151</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>985.933719206349</v>
+      </c>
+      <c r="I7" s="82"/>
+      <c r="K7" s="83">
+        <f>C7</f>
+        <v>1643.2228653439151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="4">
+        <f>РасхСосредоточПотреб!B45</f>
+        <v>13870.060832084442</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>10402.545624063332</v>
+      </c>
+      <c r="I8" s="82">
+        <f>C8</f>
+        <v>13870.060832084442</v>
+      </c>
+      <c r="K8" s="83"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="4">
+        <f>РасхСосредоточПотреб!B50</f>
+        <v>11047.236678641313</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>8285.4275089809853</v>
+      </c>
+      <c r="I9" s="82"/>
+      <c r="K9" s="83">
+        <f>C9</f>
+        <v>11047.236678641313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="4">
+        <f>SUM(C3:C9)</f>
+        <v>31143.313292468047</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <f>SUM(E3:E9)</f>
+        <v>23334.091604059675</v>
+      </c>
+      <c r="I10" s="82"/>
+      <c r="K10" s="83"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="I11" s="76">
+        <f>SUM(I2:I8)</f>
+        <v>16200.718707089083</v>
+      </c>
+      <c r="K11" s="77">
+        <f>SUM(K2:K10)</f>
+        <v>13561.030144650613</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15">
+        <v>0.6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <f>0.59*(E3+E4+E8+E9)</f>
+        <v>12544.064395983345</v>
+      </c>
+      <c r="E16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16">
+        <v>0.23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16">
+        <v>11936</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18">
+        <f>(POWER(F15,2)+POWER(F16,2))/(1.1*I16/1000)</f>
+        <v>3.1448025834755054E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>B18*1000</f>
+        <v>31.448025834755054</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Gas Round Calculation
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6687095D-8156-4B72-945E-8D902D9C7693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FABE397-1391-468E-B806-E036A93B5A93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="РасхСосредоточПотреб" sheetId="6" r:id="rId6"/>
     <sheet name="РасчРасхСосредоточПотр" sheetId="7" r:id="rId7"/>
     <sheet name="ЧасовыеРасходы" sheetId="8" r:id="rId8"/>
+    <sheet name="КольцевойРасчет" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="193">
   <si>
     <t>CH4</t>
   </si>
@@ -499,6 +500,135 @@
   </si>
   <si>
     <t>325-426</t>
+  </si>
+  <si>
+    <t>м</t>
+  </si>
+  <si>
+    <t>№ участка</t>
+  </si>
+  <si>
+    <t>расчетная Lp=1.1L</t>
+  </si>
+  <si>
+    <t>Расчетный расход газа на участке Vp, м3/ч</t>
+  </si>
+  <si>
+    <t>Диаметр газопровода Dн×δ, мм</t>
+  </si>
+  <si>
+    <t>Среднеквадратичное падение давления А, МПа2 /км</t>
+  </si>
+  <si>
+    <t>Фактическое среднеквадратичное паде-ние давления Аф, МПа2/км</t>
+  </si>
+  <si>
+    <t>Среднеквадратичные потери давления Аф×Lp, МПа2</t>
+  </si>
+  <si>
+    <t>в начале участка Рн</t>
+  </si>
+  <si>
+    <t>в конце участка Рк</t>
+  </si>
+  <si>
+    <t>Давление газа, Мпа</t>
+  </si>
+  <si>
+    <t>Аварийный режим 1</t>
+  </si>
+  <si>
+    <t>ГРС-1</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>Длина участка, км</t>
+  </si>
+  <si>
+    <t>по плану, км</t>
+  </si>
+  <si>
+    <t>Аварийный режим 2</t>
+  </si>
+  <si>
+    <t>8-ГРП2</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>8-7</t>
+  </si>
+  <si>
+    <t>7-6</t>
+  </si>
+  <si>
+    <t>6-5</t>
+  </si>
+  <si>
+    <t>5-4</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>2-ГРП1</t>
+  </si>
+  <si>
+    <t>Полукольцо ГРС-1-2-3-4-РК1</t>
+  </si>
+  <si>
+    <t>4-РК1</t>
+  </si>
+  <si>
+    <t>Нормальный режим</t>
+  </si>
+  <si>
+    <t>Полукольцо ГРС-1-8-7-6-5-РК2</t>
+  </si>
+  <si>
+    <t>5-РК2</t>
+  </si>
+  <si>
+    <t>Расчет ответвлений</t>
+  </si>
+  <si>
+    <t>3-ХЗ</t>
+  </si>
+  <si>
+    <t>6-Б</t>
+  </si>
+  <si>
+    <t>7-БПК</t>
+  </si>
+  <si>
+    <t>426x9</t>
+  </si>
+  <si>
+    <t>325x8</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1151,6 +1281,27 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1220,33 +1371,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1848,7 +1995,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,36 +2101,36 @@
         <f>E2</f>
         <v>897</v>
       </c>
-      <c r="J2" s="44">
+      <c r="J2" s="59">
         <v>5</v>
       </c>
-      <c r="K2" s="44">
+      <c r="K2" s="59">
         <v>6</v>
       </c>
-      <c r="L2" s="44">
+      <c r="L2" s="59">
         <v>7</v>
       </c>
-      <c r="M2" s="44">
+      <c r="M2" s="59">
         <v>8</v>
       </c>
-      <c r="N2" s="46">
+      <c r="N2" s="61">
         <v>9</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="44">
+      <c r="Q2" s="59">
         <v>5</v>
       </c>
-      <c r="R2" s="44">
+      <c r="R2" s="59">
         <v>6</v>
       </c>
-      <c r="S2" s="44">
+      <c r="S2" s="59">
         <v>7</v>
       </c>
-      <c r="T2" s="44">
+      <c r="T2" s="59">
         <v>8</v>
       </c>
-      <c r="U2" s="46">
+      <c r="U2" s="61">
         <v>9</v>
       </c>
     </row>
@@ -2013,18 +2160,18 @@
         <f t="shared" ref="I3:I28" si="2">E3</f>
         <v>1670</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="47"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="62"/>
       <c r="O3" s="11"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="47"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="62"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -2052,18 +2199,18 @@
         <f t="shared" si="2"/>
         <v>1899</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="47"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="62"/>
       <c r="O4" s="11"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="47"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="62"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -2091,18 +2238,18 @@
         <f t="shared" si="2"/>
         <v>3707</v>
       </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="47"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="62"/>
       <c r="O5" s="11"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="47"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="62"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -2130,18 +2277,18 @@
         <f t="shared" si="2"/>
         <v>5032</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="47"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="62"/>
       <c r="O6" s="11"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="47"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="62"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -2163,11 +2310,11 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="47"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="62"/>
       <c r="O7" s="25">
         <f>B7</f>
         <v>7</v>
@@ -2176,11 +2323,11 @@
         <f t="shared" ref="P7:P12" si="3">E7</f>
         <v>5824</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="47"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="62"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -2202,11 +2349,11 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="47"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="62"/>
       <c r="O8" s="25">
         <f t="shared" ref="O8:O12" si="4">B8</f>
         <v>8</v>
@@ -2215,11 +2362,11 @@
         <f t="shared" si="3"/>
         <v>2793</v>
       </c>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="47"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="62"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -2241,11 +2388,11 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="47"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="62"/>
       <c r="O9" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2254,11 +2401,11 @@
         <f t="shared" si="3"/>
         <v>3476</v>
       </c>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="47"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="62"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -2280,11 +2427,11 @@
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="47"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="62"/>
       <c r="O10" s="25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -2293,11 +2440,11 @@
         <f t="shared" si="3"/>
         <v>1348</v>
       </c>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="47"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="62"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -2319,11 +2466,11 @@
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="47"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="62"/>
       <c r="O11" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2332,11 +2479,11 @@
         <f t="shared" si="3"/>
         <v>4547</v>
       </c>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="47"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="62"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -2358,11 +2505,11 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="47"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="62"/>
       <c r="O12" s="25">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -2371,11 +2518,11 @@
         <f t="shared" si="3"/>
         <v>2048</v>
       </c>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="47"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="62"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -2403,18 +2550,18 @@
         <f t="shared" si="2"/>
         <v>3178</v>
       </c>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="47"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="62"/>
       <c r="O13" s="11"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="47"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="62"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -2442,18 +2589,18 @@
         <f t="shared" si="2"/>
         <v>1806</v>
       </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="47"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="62"/>
       <c r="O14" s="11"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="47"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="62"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -2481,18 +2628,18 @@
         <f t="shared" si="2"/>
         <v>1853</v>
       </c>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="47"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="62"/>
       <c r="O15" s="11"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="47"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="62"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -2520,18 +2667,18 @@
         <f t="shared" si="2"/>
         <v>1057</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="47"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="62"/>
       <c r="O16" s="11"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="47"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="62"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -2559,18 +2706,18 @@
         <f t="shared" si="2"/>
         <v>1757</v>
       </c>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="47"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="62"/>
       <c r="O17" s="11"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="47"/>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="62"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -2598,18 +2745,18 @@
         <f t="shared" si="2"/>
         <v>2128</v>
       </c>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="47"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="62"/>
       <c r="O18" s="11"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="47"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="62"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -2637,18 +2784,18 @@
         <f t="shared" si="2"/>
         <v>4505</v>
       </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="47"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="62"/>
       <c r="O19" s="11"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="47"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="62"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2676,18 +2823,18 @@
         <f t="shared" si="2"/>
         <v>3329</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="47"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="62"/>
       <c r="O20" s="11"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="47"/>
+      <c r="Q20" s="60"/>
+      <c r="R20" s="60"/>
+      <c r="S20" s="60"/>
+      <c r="T20" s="60"/>
+      <c r="U20" s="62"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -2709,11 +2856,11 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="47"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="62"/>
       <c r="O21" s="25">
         <f>B21</f>
         <v>5</v>
@@ -2722,11 +2869,11 @@
         <f>E21</f>
         <v>2156</v>
       </c>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="47"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="60"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="62"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -2748,11 +2895,11 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="47"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="62"/>
       <c r="O22" s="25">
         <f t="shared" ref="O22:O25" si="6">B22</f>
         <v>8</v>
@@ -2761,11 +2908,11 @@
         <f>E22</f>
         <v>1645</v>
       </c>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="47"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="62"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2787,11 +2934,11 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="47"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="62"/>
       <c r="O23" s="25">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -2800,11 +2947,11 @@
         <f>E23</f>
         <v>1551</v>
       </c>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="47"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="62"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -2826,11 +2973,11 @@
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="47"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="62"/>
       <c r="O24" s="25">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -2839,11 +2986,11 @@
         <f>E24</f>
         <v>4816</v>
       </c>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="47"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="62"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -2865,11 +3012,11 @@
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="47"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="62"/>
       <c r="O25" s="25">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -2878,11 +3025,11 @@
         <f>E25</f>
         <v>5057</v>
       </c>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="47"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="62"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2910,18 +3057,18 @@
         <f t="shared" si="2"/>
         <v>4484</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="47"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="62"/>
       <c r="O26" s="11"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="47"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="60"/>
+      <c r="S26" s="60"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="62"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -2949,18 +3096,18 @@
         <f t="shared" si="2"/>
         <v>3486</v>
       </c>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="47"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="62"/>
       <c r="O27" s="11"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="47"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="62"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
@@ -2988,18 +3135,18 @@
         <f t="shared" si="2"/>
         <v>3483</v>
       </c>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="47"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="62"/>
       <c r="O28" s="17"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="47"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
+      <c r="T28" s="60"/>
+      <c r="U28" s="62"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29">
@@ -3131,7 +3278,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3373,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3268,8 +3415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33035FD5-04D2-4D7F-99BE-F176EC4254F0}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,50 +3433,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="54" t="s">
+      <c r="G1" s="72"/>
+      <c r="H1" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="69" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -3364,32 +3511,32 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
@@ -3430,18 +3577,18 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="53"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="68"/>
     </row>
     <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
@@ -3498,32 +3645,32 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="65"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
@@ -3563,18 +3710,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
     </row>
     <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
@@ -3741,7 +3888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD0AAA4-CEDA-4DBB-82AC-0AD67E237AF8}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
@@ -4117,8 +4264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9ED7318-8A47-492B-BAB1-7E25EB2B5EE2}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4128,50 +4275,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="54" t="s">
+      <c r="G1" s="72"/>
+      <c r="H1" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="69" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -4206,18 +4353,18 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
@@ -4337,32 +4484,32 @@
       <c r="B8" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="60" t="str">
+      <c r="C8" s="75" t="str">
         <f>РасхСосредоточПотреб!C6&amp;"+"&amp;РасхСосредоточПотреб!C7</f>
         <v>376.27+229.06</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="77"/>
       <c r="J8" s="30">
         <f>РасхСосредоточПотреб!B6+РасхСосредоточПотреб!B7</f>
         <v>605.33020079843004</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="59"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="41" t="s">
         <v>58</v>
       </c>
@@ -4372,18 +4519,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="65"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="80"/>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
@@ -4392,10 +4539,10 @@
       <c r="B11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="62"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="30">
         <f>РасхСосредоточПотреб!B31</f>
         <v>3484</v>
@@ -4427,10 +4574,10 @@
       <c r="B12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="62"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="30">
         <f>РасхСосредоточПотреб!B32</f>
         <v>13935</v>
@@ -4462,10 +4609,10 @@
       <c r="B13" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="30">
         <f>РасхСосредоточПотреб!B33</f>
         <v>2903</v>
@@ -4491,16 +4638,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="74"/>
       <c r="I14" s="42" t="s">
         <v>58</v>
       </c>
@@ -4510,18 +4657,18 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="65"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
@@ -4635,16 +4782,16 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="59"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="74"/>
       <c r="I19" s="41" t="s">
         <v>58</v>
       </c>
@@ -4792,8 +4939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC937C0-5E57-457A-81B6-0468CB5DE98C}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4808,48 +4955,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="54" t="s">
         <v>137</v>
       </c>
       <c r="J1" s="43"/>
-      <c r="K1" s="80" t="s">
+      <c r="K1" s="55" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
-      <c r="B2" s="68">
+      <c r="B2" s="45">
         <v>2</v>
       </c>
-      <c r="C2" s="70">
+      <c r="C2" s="47">
         <v>3</v>
       </c>
-      <c r="D2" s="68">
+      <c r="D2" s="45">
         <v>4</v>
       </c>
-      <c r="E2" s="71">
+      <c r="E2" s="48">
         <v>5</v>
       </c>
-      <c r="I2" s="78"/>
+      <c r="I2" s="53"/>
       <c r="J2" s="43"/>
-      <c r="K2" s="81"/>
+      <c r="K2" s="56"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -4869,11 +5016,11 @@
         <f>C3*D3</f>
         <v>1467.9014092600287</v>
       </c>
-      <c r="I3" s="79">
+      <c r="I3" s="54">
         <f>C3</f>
         <v>1834.8767615750357</v>
       </c>
-      <c r="K3" s="80"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -4893,8 +5040,8 @@
         <f t="shared" ref="E4:E9" si="0">C4*D4</f>
         <v>1105.2515525826791</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="K4" s="83">
+      <c r="I4" s="57"/>
+      <c r="K4" s="58">
         <f>C5</f>
         <v>870.57060066538452</v>
       </c>
@@ -4917,8 +5064,8 @@
         <f t="shared" si="0"/>
         <v>739.98501056557677</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="K5" s="83"/>
+      <c r="I5" s="57"/>
+      <c r="K5" s="58"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -4938,11 +5085,11 @@
         <f t="shared" si="0"/>
         <v>347.04677940072361</v>
       </c>
-      <c r="I6" s="82">
+      <c r="I6" s="57">
         <f>C6</f>
         <v>495.78111342960517</v>
       </c>
-      <c r="K6" s="83"/>
+      <c r="K6" s="58"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -4962,8 +5109,8 @@
         <f t="shared" si="0"/>
         <v>985.933719206349</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="K7" s="83">
+      <c r="I7" s="57"/>
+      <c r="K7" s="58">
         <f>C7</f>
         <v>1643.2228653439151</v>
       </c>
@@ -4986,11 +5133,11 @@
         <f t="shared" si="0"/>
         <v>10402.545624063332</v>
       </c>
-      <c r="I8" s="82">
+      <c r="I8" s="57">
         <f>C8</f>
         <v>13870.060832084442</v>
       </c>
-      <c r="K8" s="83"/>
+      <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -5010,17 +5157,17 @@
         <f t="shared" si="0"/>
         <v>8285.4275089809853</v>
       </c>
-      <c r="I9" s="82"/>
-      <c r="K9" s="83">
+      <c r="I9" s="57"/>
+      <c r="K9" s="58">
         <f>C9</f>
         <v>11047.236678641313</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="75"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="4">
         <f>SUM(C3:C9)</f>
         <v>31143.313292468047</v>
@@ -5030,8 +5177,8 @@
         <f>SUM(E3:E9)</f>
         <v>23334.091604059675</v>
       </c>
-      <c r="I10" s="82"/>
-      <c r="K10" s="83"/>
+      <c r="I10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
@@ -5039,11 +5186,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="I11" s="76">
+      <c r="I11" s="51">
         <f>SUM(I2:I8)</f>
         <v>16200.718707089083</v>
       </c>
-      <c r="K11" s="77">
+      <c r="K11" s="52">
         <f>SUM(K2:K10)</f>
         <v>13561.030144650613</v>
       </c>
@@ -5074,13 +5221,16 @@
         <v>144</v>
       </c>
       <c r="F16">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="H16" t="s">
         <v>146</v>
       </c>
       <c r="I16">
         <v>11936</v>
+      </c>
+      <c r="J16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5094,7 +5244,7 @@
       </c>
       <c r="B18">
         <f>(POWER(F15,2)+POWER(F16,2))/(1.1*I16/1000)</f>
-        <v>3.1448025834755054E-2</v>
+        <v>3.2179198147696805E-2</v>
       </c>
       <c r="C18" t="s">
         <v>147</v>
@@ -5103,7 +5253,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <f>B18*1000</f>
-        <v>31.448025834755054</v>
+        <v>32.179198147696802</v>
       </c>
       <c r="C19" t="s">
         <v>148</v>
@@ -5121,4 +5271,1343 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECA6797-C0EB-4566-9FAB-3CEBA037D098}">
+  <dimension ref="A1:J46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="86"/>
+      <c r="D1" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="84" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="84" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="86"/>
+    </row>
+    <row r="2" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="87"/>
+      <c r="B2" s="88" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="88" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <f>1.1*B5</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D5" s="4">
+        <v>23334.09</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
+        <f>C5*G5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J5" s="4">
+        <f>I5-H5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:C13" si="0">1.1*B6</f>
+        <v>1.0461</v>
+      </c>
+      <c r="D6" s="4">
+        <v>23334.09</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:H10" si="1">C6*G6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <f>J5</f>
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:J10" si="2">I6-H6</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="90" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.73920000000000008</v>
+      </c>
+      <c r="D7" s="4">
+        <v>22228.84</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:I13" si="3">J6</f>
+        <v>0.6</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.224</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3464</v>
+      </c>
+      <c r="D8" s="4">
+        <v>21242.91</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="90" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20502.919999999998</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.379</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5169000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12217.49</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="89" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2517000000000005</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1814.95</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
+        <f t="shared" ref="H11:H13" si="4">C11*G11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ref="J11:J13" si="5">I11-H11</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4421000000000002</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1467.9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="89" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1.032</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1352000000000002</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1467.9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="68"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="4">
+        <f>1.1*B15</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D15" s="4">
+        <v>23334.09</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
+        <f>C15*G15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J15" s="4">
+        <f>I15-H15</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1.08</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:C23" si="6">1.1*B16</f>
+        <v>1.1880000000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>23334.09</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <f t="shared" ref="H16:H20" si="7">C16*G16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <f>J15</f>
+        <v>0.6</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" ref="J16:J20" si="8">I16-H16</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="6"/>
+        <v>1.4421000000000002</v>
+      </c>
+      <c r="D17" s="4">
+        <v>21866.19</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" ref="I17:I23" si="9">J16</f>
+        <v>0.6</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="6"/>
+        <v>2.2517000000000005</v>
+      </c>
+      <c r="D18" s="4">
+        <v>21519.14</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1.379</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="6"/>
+        <v>1.5169000000000001</v>
+      </c>
+      <c r="D19" s="4">
+        <v>11116.6</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="6"/>
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2831.17</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.224</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="6"/>
+        <v>1.3464</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2091.1799999999998</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
+        <f t="shared" ref="H21:H23" si="10">C21*G21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" ref="J21:J23" si="11">I21-H21</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="6"/>
+        <v>0.73920000000000008</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1105.25</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="11"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="6"/>
+        <v>0.62039999999999995</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1105.25</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="11"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="68"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="68"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="4">
+        <f>1.1*B26</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D26" s="4">
+        <v>31143.3</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4">
+        <f>C26*G26</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J26" s="4">
+        <f>I26-H26</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1.08</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" ref="C27:C30" si="12">1.1*B27</f>
+        <v>1.1880000000000002</v>
+      </c>
+      <c r="D27" s="4">
+        <v>16200.71</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4">
+        <f t="shared" ref="H27:H30" si="13">C27*G27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <f>J26</f>
+        <v>0.6</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ref="J27:J30" si="14">I27-H27</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="12"/>
+        <v>1.4421000000000002</v>
+      </c>
+      <c r="D28" s="4">
+        <v>14365.84</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" ref="I28:I30" si="15">J27</f>
+        <v>0.6</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="14"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="12"/>
+        <v>2.2517000000000005</v>
+      </c>
+      <c r="D29" s="4">
+        <v>13870.06</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="15"/>
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="14"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="90" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="12"/>
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="D30" s="4">
+        <v>13870.06</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="15"/>
+        <v>0.6</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="14"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="68"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="68"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="4">
+        <f>1.1*B33</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D33" s="4">
+        <v>31143.3</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4">
+        <f>C33*G33</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J33" s="4">
+        <f>I33-H33</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" ref="C34:C38" si="16">1.1*B34</f>
+        <v>1.0461</v>
+      </c>
+      <c r="D34" s="4">
+        <v>14942.59</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4">
+        <f t="shared" ref="H34:H38" si="17">C34*G34</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <f>J33</f>
+        <v>0.6</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" ref="J34:J38" si="18">I34-H34</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="90" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="16"/>
+        <v>0.73920000000000008</v>
+      </c>
+      <c r="D35" s="4">
+        <v>13561.03</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" ref="I35:I37" si="19">J34</f>
+        <v>0.6</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="18"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1.224</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="16"/>
+        <v>1.3464</v>
+      </c>
+      <c r="D36" s="4">
+        <v>11917.81</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="19"/>
+        <v>0.6</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="18"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="89" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="16"/>
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="D37" s="4">
+        <v>11047.24</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4">
+        <f t="shared" ref="H37" si="20">C37*G37</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <f t="shared" si="19"/>
+        <v>0.6</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" ref="J37" si="21">I37-H37</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="90" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="16"/>
+        <v>0.29590000000000005</v>
+      </c>
+      <c r="D38" s="4">
+        <v>11047.24</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <f>J36</f>
+        <v>0.6</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="18"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="66" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="68"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1.032</v>
+      </c>
+      <c r="C40" s="4">
+        <f>1.1*B40</f>
+        <v>1.1352000000000002</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1834.87</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4">
+        <f>C40*G40</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4">
+        <f>I40-H40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" ref="C41:C46" si="22">1.1*B41</f>
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="D41" s="4">
+        <v>495.78</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
+        <f t="shared" ref="H41:H45" si="23">C41*G41</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4">
+        <f t="shared" ref="J41:J45" si="24">I41-H41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="90" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="22"/>
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>13870.06</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="22"/>
+        <v>0.29590000000000005</v>
+      </c>
+      <c r="D43" s="4">
+        <v>11047.24</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="90" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="22"/>
+        <v>0.32780000000000004</v>
+      </c>
+      <c r="D44" s="4">
+        <v>870.57</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="89" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="4">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="22"/>
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1643.22</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="89" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="22"/>
+        <v>0.62039999999999995</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1381.56</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4">
+        <f t="shared" ref="H46" si="25">C46*G46</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4">
+        <f t="shared" ref="J46" si="26">I46-H46</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update gidravlic calculation and blueprint
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FABE397-1391-468E-B806-E036A93B5A93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F32671E-7E2B-46F9-B267-2ABF6E1A9743}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="193">
   <si>
     <t>CH4</t>
   </si>
@@ -499,9 +499,6 @@
     <t>Па/м</t>
   </si>
   <si>
-    <t>325-426</t>
-  </si>
-  <si>
     <t>м</t>
   </si>
   <si>
@@ -625,10 +622,13 @@
     <t>7-БПК</t>
   </si>
   <si>
-    <t>426x9</t>
-  </si>
-  <si>
     <t>325x8</t>
+  </si>
+  <si>
+    <t>108x4</t>
+  </si>
+  <si>
+    <t>76x3</t>
   </si>
 </sst>
 </file>
@@ -1302,6 +1302,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,23 +1382,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1680,17 +1680,17 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>8</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>1.9801077682981592</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1854,13 +1854,13 @@
         <v>1.2523447967842787</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>SUM(B2:B8)</f>
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0.73337724555280348</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>36021.945</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>14.930213115639303</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>9.6366200000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>9.7037756774560009</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>10.674153245201602</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>1.0125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>2.0052387124520159</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>0.2023690200000002</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>8.3802227800000022</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1998,25 +1998,25 @@
       <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="16" max="16" width="25.85546875" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.88671875" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2101,40 +2101,40 @@
         <f>E2</f>
         <v>897</v>
       </c>
-      <c r="J2" s="59">
+      <c r="J2" s="62">
         <v>5</v>
       </c>
-      <c r="K2" s="59">
+      <c r="K2" s="62">
         <v>6</v>
       </c>
-      <c r="L2" s="59">
+      <c r="L2" s="62">
         <v>7</v>
       </c>
-      <c r="M2" s="59">
+      <c r="M2" s="62">
         <v>8</v>
       </c>
-      <c r="N2" s="61">
+      <c r="N2" s="64">
         <v>9</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="59">
+      <c r="Q2" s="62">
         <v>5</v>
       </c>
-      <c r="R2" s="59">
+      <c r="R2" s="62">
         <v>6</v>
       </c>
-      <c r="S2" s="59">
+      <c r="S2" s="62">
         <v>7</v>
       </c>
-      <c r="T2" s="59">
+      <c r="T2" s="62">
         <v>8</v>
       </c>
-      <c r="U2" s="61">
+      <c r="U2" s="64">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2160,20 +2160,20 @@
         <f t="shared" ref="I3:I28" si="2">E3</f>
         <v>1670</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="11"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="62"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="65"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2199,20 +2199,20 @@
         <f t="shared" si="2"/>
         <v>1899</v>
       </c>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="62"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="65"/>
       <c r="O4" s="11"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="62"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="65"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2238,20 +2238,20 @@
         <f t="shared" si="2"/>
         <v>3707</v>
       </c>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="62"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="65"/>
       <c r="O5" s="11"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="62"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="65"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2277,20 +2277,20 @@
         <f t="shared" si="2"/>
         <v>5032</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="62"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="11"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="62"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="65"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2310,11 +2310,11 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="62"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="25">
         <f>B7</f>
         <v>7</v>
@@ -2323,13 +2323,13 @@
         <f t="shared" ref="P7:P12" si="3">E7</f>
         <v>5824</v>
       </c>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="62"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="65"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2349,11 +2349,11 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="62"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25">
         <f t="shared" ref="O8:O12" si="4">B8</f>
         <v>8</v>
@@ -2362,13 +2362,13 @@
         <f t="shared" si="3"/>
         <v>2793</v>
       </c>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="60"/>
-      <c r="U8" s="62"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="65"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2388,11 +2388,11 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="62"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="65"/>
       <c r="O9" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2401,13 +2401,13 @@
         <f t="shared" si="3"/>
         <v>3476</v>
       </c>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="62"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="65"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2427,11 +2427,11 @@
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="62"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="65"/>
       <c r="O10" s="25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -2440,13 +2440,13 @@
         <f t="shared" si="3"/>
         <v>1348</v>
       </c>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="62"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="65"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2466,11 +2466,11 @@
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="62"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="65"/>
       <c r="O11" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2479,13 +2479,13 @@
         <f t="shared" si="3"/>
         <v>4547</v>
       </c>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="62"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="65"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2505,11 +2505,11 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="62"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="65"/>
       <c r="O12" s="25">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -2518,13 +2518,13 @@
         <f t="shared" si="3"/>
         <v>2048</v>
       </c>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="62"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="65"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2550,20 +2550,20 @@
         <f t="shared" si="2"/>
         <v>3178</v>
       </c>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="65"/>
       <c r="O13" s="11"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="62"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="65"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2589,20 +2589,20 @@
         <f t="shared" si="2"/>
         <v>1806</v>
       </c>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="65"/>
       <c r="O14" s="11"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="60"/>
-      <c r="U14" s="62"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="65"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2628,20 +2628,20 @@
         <f t="shared" si="2"/>
         <v>1853</v>
       </c>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="62"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="65"/>
       <c r="O15" s="11"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="62"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="65"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2667,20 +2667,20 @@
         <f t="shared" si="2"/>
         <v>1057</v>
       </c>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="62"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="65"/>
       <c r="O16" s="11"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="62"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="65"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2706,20 +2706,20 @@
         <f t="shared" si="2"/>
         <v>1757</v>
       </c>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="62"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="65"/>
       <c r="O17" s="11"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="60"/>
-      <c r="U17" s="62"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="65"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2745,20 +2745,20 @@
         <f t="shared" si="2"/>
         <v>2128</v>
       </c>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="62"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="65"/>
       <c r="O18" s="11"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="62"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="65"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2784,20 +2784,20 @@
         <f t="shared" si="2"/>
         <v>4505</v>
       </c>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="62"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="65"/>
       <c r="O19" s="11"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="60"/>
-      <c r="U19" s="62"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="63"/>
+      <c r="U19" s="65"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2823,20 +2823,20 @@
         <f t="shared" si="2"/>
         <v>3329</v>
       </c>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="62"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="65"/>
       <c r="O20" s="11"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="62"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="63"/>
+      <c r="U20" s="65"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2856,11 +2856,11 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="62"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="65"/>
       <c r="O21" s="25">
         <f>B21</f>
         <v>5</v>
@@ -2869,13 +2869,13 @@
         <f>E21</f>
         <v>2156</v>
       </c>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="60"/>
-      <c r="U21" s="62"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="63"/>
+      <c r="U21" s="65"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2895,11 +2895,11 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="62"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="65"/>
       <c r="O22" s="25">
         <f t="shared" ref="O22:O25" si="6">B22</f>
         <v>8</v>
@@ -2908,13 +2908,13 @@
         <f>E22</f>
         <v>1645</v>
       </c>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="60"/>
-      <c r="T22" s="60"/>
-      <c r="U22" s="62"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="63"/>
+      <c r="U22" s="65"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2934,11 +2934,11 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="65"/>
       <c r="O23" s="25">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -2947,13 +2947,13 @@
         <f>E23</f>
         <v>1551</v>
       </c>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="62"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="65"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2973,11 +2973,11 @@
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="62"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="65"/>
       <c r="O24" s="25">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -2986,13 +2986,13 @@
         <f>E24</f>
         <v>4816</v>
       </c>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="62"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q24" s="63"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="63"/>
+      <c r="U24" s="65"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3012,11 +3012,11 @@
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="62"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="65"/>
       <c r="O25" s="25">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -3025,13 +3025,13 @@
         <f>E25</f>
         <v>5057</v>
       </c>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="62"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="65"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -3057,20 +3057,20 @@
         <f t="shared" si="2"/>
         <v>4484</v>
       </c>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="62"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="65"/>
       <c r="O26" s="11"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="62"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q26" s="63"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="65"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3096,20 +3096,20 @@
         <f t="shared" si="2"/>
         <v>3486</v>
       </c>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="62"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="65"/>
       <c r="O27" s="11"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="60"/>
-      <c r="T27" s="60"/>
-      <c r="U27" s="62"/>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="65"/>
+    </row>
+    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3135,20 +3135,20 @@
         <f t="shared" si="2"/>
         <v>3483</v>
       </c>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="65"/>
       <c r="O28" s="17"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="62"/>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="65"/>
+    </row>
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29">
         <f>SUM(C2:C28)</f>
         <v>234.82999999999996</v>
@@ -3214,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J30">
         <f>SUMIF($H$2:$H$28,J2,$I$2:$I$28)</f>
         <v>6032</v>
@@ -3281,9 +3281,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3376,12 +3376,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3419,66 +3419,66 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="69" t="s">
+      <c r="G1" s="75"/>
+      <c r="H1" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="72" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -3510,35 +3510,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
-    </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
+    </row>
+    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -3576,21 +3576,21 @@
       </c>
       <c r="L6" s="32"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="68"/>
-    </row>
-    <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="71"/>
+    </row>
+    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>2</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>1264.8223659807281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -3644,35 +3644,35 @@
         <v>1834.8767615750357</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="65"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="68"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="68"/>
-    </row>
-    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
+    </row>
+    <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>1</v>
       </c>
@@ -3709,21 +3709,21 @@
         <v>331.14565685717059</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
-    </row>
-    <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
+    </row>
+    <row r="14" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>2</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>1050.4187838711782</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -3777,7 +3777,7 @@
         <v>1381.5644407283489</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -3789,7 +3789,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -3801,7 +3801,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
@@ -3813,7 +3813,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -3825,7 +3825,7 @@
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -3837,7 +3837,7 @@
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -3849,7 +3849,7 @@
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -3892,15 +3892,15 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -3924,12 +3924,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E8" s="39" t="s">
         <v>31</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" s="39" t="s">
         <v>69</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>52&amp;"*"&amp;0.05&amp;"*"&amp;'расчетКол-ваЖит'!E29</f>
         <v>52*0.05*79532</v>
@@ -4013,7 +4013,7 @@
         <v>206783.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>58</v>
       </c>
@@ -4103,12 +4103,12 @@
         <v>8426</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>3484</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>13935</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -4135,12 +4135,12 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>115</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>118</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>796878</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>13870.060832084442</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="E46" t="s">
         <v>114</v>
@@ -4217,7 +4217,7 @@
         <v>634698</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>111</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>67119.313500000004</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>133</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>8054.3176200000007</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>134</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>13258.136</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>135</v>
       </c>
@@ -4268,59 +4268,59 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="69" t="s">
+      <c r="G1" s="75"/>
+      <c r="H1" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="72" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -4352,21 +4352,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>1</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>47.131763089910272</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>135.50381888349202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>3</v>
       </c>
@@ -4477,39 +4477,39 @@
         <v>82.604817893552152</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>4</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="75" t="str">
+      <c r="C8" s="78" t="str">
         <f>РасхСосредоточПотреб!C6&amp;"+"&amp;РасхСосредоточПотреб!C7</f>
         <v>376.27+229.06</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="77"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
       <c r="J8" s="30">
         <f>РасхСосредоточПотреб!B6+РасхСосредоточПотреб!B7</f>
         <v>605.33020079843004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="73" t="s">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="41" t="s">
         <v>58</v>
       </c>
@@ -4518,31 +4518,31 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="80"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="83"/>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>1</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="77"/>
+      <c r="D11" s="80"/>
       <c r="E11" s="30">
         <f>РасхСосредоточПотреб!B31</f>
         <v>3484</v>
@@ -4567,17 +4567,17 @@
         <v>40.299508165554819</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>2</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="77"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="30">
         <f>РасхСосредоточПотреб!B32</f>
         <v>13935</v>
@@ -4602,17 +4602,17 @@
         <v>351.38649509347704</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>3</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="77"/>
+      <c r="D13" s="80"/>
       <c r="E13" s="30">
         <f>РасхСосредоточПотреб!B33</f>
         <v>2903</v>
@@ -4637,17 +4637,17 @@
         <v>104.09511017057334</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="73" t="s">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="74"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="77"/>
       <c r="I14" s="42" t="s">
         <v>58</v>
       </c>
@@ -4656,21 +4656,21 @@
         <v>495.78111342960517</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="65"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="30">
         <v>1</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>85.044125596627694</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="30">
         <v>2</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>106.30515699578461</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>3</v>
       </c>
@@ -4781,17 +4781,17 @@
         <v>1451.8735827515029</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77"/>
       <c r="I19" s="41" t="s">
         <v>58</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>1643.2228653439151</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
@@ -4812,7 +4812,7 @@
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
@@ -4824,7 +4824,7 @@
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="B22" s="43"/>
       <c r="C22" s="43"/>
@@ -4836,7 +4836,7 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -4848,7 +4848,7 @@
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
@@ -4860,7 +4860,7 @@
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
@@ -4872,7 +4872,7 @@
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="43"/>
       <c r="C26" s="43"/>
@@ -4884,7 +4884,7 @@
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -4896,7 +4896,7 @@
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="43"/>
       <c r="C28" s="43"/>
@@ -4940,21 +4940,21 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>125</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="J2" s="43"/>
       <c r="K2" s="56"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5067,7 +5067,7 @@
       <c r="I5" s="57"/>
       <c r="K5" s="58"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -5091,7 +5091,7 @@
       </c>
       <c r="K6" s="58"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>1643.2228653439151</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -5163,11 +5163,11 @@
         <v>11047.236678641313</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="83"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="4">
         <f>SUM(C3:C9)</f>
         <v>31143.313292468047</v>
@@ -5180,7 +5180,7 @@
       <c r="I10" s="57"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5195,7 +5195,7 @@
         <v>13561.030144650613</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -5209,13 +5209,13 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
       <c r="B16">
-        <f>0.59*(E3+E4+E8+E9)</f>
-        <v>12544.064395983345</v>
+        <f>0.59*SUM(E10)</f>
+        <v>13767.114046395207</v>
       </c>
       <c r="E16" t="s">
         <v>144</v>
@@ -5230,15 +5230,15 @@
         <v>11936</v>
       </c>
       <c r="J16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19">
         <f>B18*1000</f>
         <v>32.179198147696802</v>
@@ -5259,9 +5259,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>149</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5275,63 +5275,63 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECA6797-C0EB-4566-9FAB-3CEBA037D098}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="88"/>
+      <c r="D1" s="89" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="89" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="87" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="88"/>
+    </row>
+    <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="90"/>
+      <c r="B2" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="85" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="84" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="84" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="84" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="85" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" s="86"/>
-    </row>
-    <row r="2" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="88" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="88" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88" t="s">
+      <c r="J2" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="J2" s="88" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -5363,23 +5363,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="B5" s="4">
         <v>0.5</v>
@@ -5392,25 +5392,33 @@
         <v>23334.09</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="H5" s="4">
         <f>C5*G5</f>
-        <v>0</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="I5" s="4">
         <v>0.6</v>
       </c>
       <c r="J5" s="4">
         <f>I5-H5</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>174</v>
+        <v>0.58019999999999994</v>
+      </c>
+      <c r="M5">
+        <f>D5*gazProperties!$B$13/0.73</f>
+        <v>23442.041988604407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="60" t="s">
+        <v>173</v>
       </c>
       <c r="B6" s="4">
         <v>0.95099999999999996</v>
@@ -5423,26 +5431,34 @@
         <v>23334.09</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="H6" s="4">
         <f t="shared" ref="H6:H10" si="1">C6*G6</f>
-        <v>0</v>
+        <v>3.7659600000000001E-2</v>
       </c>
       <c r="I6" s="4">
         <f>J5</f>
-        <v>0.6</v>
+        <v>0.58019999999999994</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" ref="J6:J10" si="2">I6-H6</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="90" t="s">
-        <v>175</v>
+        <v>0.54254039999999992</v>
+      </c>
+      <c r="M6">
+        <f>D6*gazProperties!$B$13/0.73</f>
+        <v>23442.041988604407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="61" t="s">
+        <v>174</v>
       </c>
       <c r="B7" s="4">
         <v>0.67200000000000004</v>
@@ -5455,26 +5471,34 @@
         <v>22228.84</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="H7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5872000000000006E-2</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" ref="I7:I13" si="3">J6</f>
-        <v>0.6</v>
+        <v>0.54254039999999992</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="89" t="s">
-        <v>176</v>
+        <v>0.51666839999999992</v>
+      </c>
+      <c r="M7">
+        <f>D7*gazProperties!$B$13/0.73</f>
+        <v>22331.678700046548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="60" t="s">
+        <v>175</v>
       </c>
       <c r="B8" s="4">
         <v>1.224</v>
@@ -5487,26 +5511,34 @@
         <v>21242.91</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
       <c r="H8" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.5777600000000002E-2</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.51666839999999992</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="90" t="s">
-        <v>177</v>
+        <v>0.47089079999999994</v>
+      </c>
+      <c r="M8">
+        <f>D8*gazProperties!$B$13/0.73</f>
+        <v>21341.187429213842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="61" t="s">
+        <v>176</v>
       </c>
       <c r="B9" s="4">
         <v>1.42</v>
@@ -5519,26 +5551,34 @@
         <v>20502.919999999998</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="H9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.1546000000000002E-2</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.47089079999999994</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="89" t="s">
-        <v>178</v>
+        <v>0.41934479999999996</v>
+      </c>
+      <c r="M9">
+        <f>D9*gazProperties!$B$13/0.73</f>
+        <v>20597.773966286964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="60" t="s">
+        <v>177</v>
       </c>
       <c r="B10" s="4">
         <v>1.379</v>
@@ -5551,26 +5591,34 @@
         <v>12217.49</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>8.6E-3</v>
+      </c>
       <c r="H10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.3045340000000001E-2</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.41934479999999996</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="89" t="s">
-        <v>179</v>
+        <v>0.40629945999999995</v>
+      </c>
+      <c r="M10">
+        <f>D10*gazProperties!$B$13/0.73</f>
+        <v>12274.01255310811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="60" t="s">
+        <v>178</v>
       </c>
       <c r="B11" s="4">
         <v>2.0470000000000002</v>
@@ -5583,26 +5631,34 @@
         <v>1814.95</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2.41E-4</v>
+      </c>
       <c r="H11" s="4">
         <f t="shared" ref="H11:H13" si="4">C11*G11</f>
-        <v>0</v>
+        <v>5.4265970000000015E-4</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.40629945999999995</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" ref="J11:J13" si="5">I11-H11</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
-        <v>180</v>
+        <v>0.40575680029999994</v>
+      </c>
+      <c r="M11">
+        <f>D11*gazProperties!$B$13/0.73</f>
+        <v>1823.3466189261105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="60" t="s">
+        <v>179</v>
       </c>
       <c r="B12" s="4">
         <v>1.3109999999999999</v>
@@ -5615,26 +5671,33 @@
         <v>1467.9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2.2599999999999999E-4</v>
+      </c>
       <c r="H12" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.40575680029999994</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="89" t="s">
-        <v>181</v>
+        <v>0.40551680029999992</v>
+      </c>
+      <c r="M12">
+        <f>D12*gazProperties!$B$13/0.73</f>
+        <v>1474.6910393793978</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="60" t="s">
+        <v>180</v>
       </c>
       <c r="B13" s="4">
         <v>1.032</v>
@@ -5647,40 +5710,48 @@
         <v>1467.9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="H13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.8813600000000006E-2</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="3"/>
-        <v>0.6</v>
+        <v>0.40551680029999992</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="68"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.35670320029999991</v>
+      </c>
+      <c r="M13">
+        <f>D13*gazProperties!$B$13/0.73</f>
+        <v>1474.6910393793978</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="4">
         <v>0.5</v>
@@ -5693,25 +5764,33 @@
         <v>23334.09</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F15" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="H15" s="4">
         <f>C15*G15</f>
-        <v>0</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="I15" s="4">
         <v>0.6</v>
       </c>
       <c r="J15" s="4">
         <f>I15-H15</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
-        <v>163</v>
+        <v>0.58019999999999994</v>
+      </c>
+      <c r="M15">
+        <f>D15*gazProperties!$B$13/0.73</f>
+        <v>23442.041988604407</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="60" t="s">
+        <v>162</v>
       </c>
       <c r="B16" s="4">
         <v>1.08</v>
@@ -5724,26 +5803,34 @@
         <v>23334.09</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="H16" s="4">
         <f t="shared" ref="H16:H20" si="7">C16*G16</f>
-        <v>0</v>
+        <v>4.2768E-2</v>
       </c>
       <c r="I16" s="4">
         <f>J15</f>
-        <v>0.6</v>
+        <v>0.58019999999999994</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" ref="J16:J20" si="8">I16-H16</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="90" t="s">
-        <v>164</v>
+        <v>0.53743199999999991</v>
+      </c>
+      <c r="M16">
+        <f>D16*gazProperties!$B$13/0.73</f>
+        <v>23442.041988604407</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="B17" s="4">
         <v>1.3109999999999999</v>
@@ -5756,26 +5843,34 @@
         <v>21866.19</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2.7E-2</v>
+      </c>
       <c r="H17" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.8936700000000005E-2</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" ref="I17:I23" si="9">J16</f>
-        <v>0.6</v>
+        <v>0.53743199999999991</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="8"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="89" t="s">
-        <v>165</v>
+        <v>0.49849529999999992</v>
+      </c>
+      <c r="M17">
+        <f>D17*gazProperties!$B$13/0.73</f>
+        <v>21967.350949225009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="60" t="s">
+        <v>164</v>
       </c>
       <c r="B18" s="4">
         <v>2.0470000000000002</v>
@@ -5788,26 +5883,34 @@
         <v>21519.14</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="H18" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.8544200000000012E-2</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.49849529999999992</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="8"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
-        <v>166</v>
+        <v>0.43995109999999993</v>
+      </c>
+      <c r="M18">
+        <f>D18*gazProperties!$B$13/0.73</f>
+        <v>21618.695369678295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="61" t="s">
+        <v>165</v>
       </c>
       <c r="B19" s="4">
         <v>1.379</v>
@@ -5820,26 +5923,34 @@
         <v>11116.6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F19" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G19" s="4">
+        <v>7.1000000000000004E-3</v>
+      </c>
       <c r="H19" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0769990000000002E-2</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.43995109999999993</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="8"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="89" t="s">
-        <v>167</v>
+        <v>0.42918110999999992</v>
+      </c>
+      <c r="M19">
+        <f>D19*gazProperties!$B$13/0.73</f>
+        <v>11168.029435496295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="B20" s="4">
         <v>1.42</v>
@@ -5852,26 +5963,34 @@
         <v>2831.17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.86E-4</v>
+      </c>
       <c r="H20" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.5913200000000004E-4</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.42918110999999992</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="8"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
-        <v>168</v>
+        <v>0.42842197799999993</v>
+      </c>
+      <c r="M20">
+        <f>D20*gazProperties!$B$13/0.73</f>
+        <v>2844.2680223174393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="60" t="s">
+        <v>167</v>
       </c>
       <c r="B21" s="4">
         <v>1.224</v>
@@ -5884,26 +6003,34 @@
         <v>2091.1799999999998</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2.9E-4</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2.9399999999999999E-4</v>
+      </c>
       <c r="H21" s="4">
         <f t="shared" ref="H21:H23" si="10">C21*G21</f>
-        <v>0</v>
+        <v>3.9584160000000001E-4</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.42842197799999993</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" ref="J21:J23" si="11">I21-H21</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="89" t="s">
-        <v>169</v>
+        <v>0.42802613639999992</v>
+      </c>
+      <c r="M21">
+        <f>D21*gazProperties!$B$13/0.73</f>
+        <v>2100.8545593905637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="60" t="s">
+        <v>168</v>
       </c>
       <c r="B22" s="4">
         <v>0.67200000000000004</v>
@@ -5916,26 +6043,34 @@
         <v>1105.25</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.1E-4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1.18E-4</v>
+      </c>
       <c r="H22" s="4">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>8.7225600000000007E-5</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.42802613639999992</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="11"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="89" t="s">
-        <v>173</v>
+        <v>0.42793891079999991</v>
+      </c>
+      <c r="M22">
+        <f>D22*gazProperties!$B$13/0.73</f>
+        <v>1110.3632885578575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="60" t="s">
+        <v>172</v>
       </c>
       <c r="B23" s="4">
         <v>0.56399999999999995</v>
@@ -5948,54 +6083,62 @@
         <v>1105.25</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="H23" s="4">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1.3648799999999997E-2</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.42793891079999991</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="11"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
-        <v>184</v>
-      </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="68"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="68"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.41429011079999989</v>
+      </c>
+      <c r="M23">
+        <f>D23*gazProperties!$B$13/0.73</f>
+        <v>1110.3632885578575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="71"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="71"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" s="4">
         <v>0.5</v>
@@ -6008,25 +6151,33 @@
         <v>31143.3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>5.2600000000000001E-2</v>
+      </c>
       <c r="H26" s="4">
         <f>C26*G26</f>
-        <v>0</v>
+        <v>2.8930000000000004E-2</v>
       </c>
       <c r="I26" s="4">
         <v>0.6</v>
       </c>
       <c r="J26" s="4">
         <f>I26-H26</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="89" t="s">
-        <v>163</v>
+        <v>0.57106999999999997</v>
+      </c>
+      <c r="M26">
+        <f>D26*gazProperties!$B$13/0.73</f>
+        <v>31287.380234828255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="60" t="s">
+        <v>162</v>
       </c>
       <c r="B27" s="4">
         <v>1.08</v>
@@ -6039,26 +6190,34 @@
         <v>16200.71</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1.67E-2</v>
+      </c>
       <c r="H27" s="4">
         <f t="shared" ref="H27:H30" si="13">C27*G27</f>
-        <v>0</v>
+        <v>1.9839600000000002E-2</v>
       </c>
       <c r="I27" s="4">
         <f>J26</f>
-        <v>0.6</v>
+        <v>0.57106999999999997</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" ref="J27:J30" si="14">I27-H27</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
-        <v>164</v>
+        <v>0.55123040000000001</v>
+      </c>
+      <c r="M27">
+        <f>D27*gazProperties!$B$13/0.73</f>
+        <v>16275.66037780789</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="B28" s="4">
         <v>1.3109999999999999</v>
@@ -6071,26 +6230,34 @@
         <v>14365.84</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0.02</v>
+      </c>
       <c r="H28" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2.8842000000000003E-2</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" ref="I28:I30" si="15">J27</f>
-        <v>0.6</v>
+        <v>0.55123040000000001</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="14"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="89" t="s">
-        <v>165</v>
+        <v>0.52238839999999997</v>
+      </c>
+      <c r="M28">
+        <f>D28*gazProperties!$B$13/0.73</f>
+        <v>14432.301601715462</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="60" t="s">
+        <v>164</v>
       </c>
       <c r="B29" s="4">
         <v>2.0470000000000002</v>
@@ -6103,26 +6270,34 @@
         <v>13870.06</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
       <c r="H29" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2.9272100000000006E-2</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" si="15"/>
-        <v>0.6</v>
+        <v>0.52238839999999997</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="14"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="90" t="s">
-        <v>183</v>
+        <v>0.49311629999999995</v>
+      </c>
+      <c r="M29">
+        <f>D29*gazProperties!$B$13/0.73</f>
+        <v>13934.22794308509</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="61" t="s">
+        <v>182</v>
       </c>
       <c r="B30" s="4">
         <v>7.9000000000000001E-2</v>
@@ -6135,54 +6310,62 @@
         <v>13870.06</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2.7E-2</v>
+      </c>
       <c r="H30" s="4">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2.3462999999999999E-3</v>
       </c>
       <c r="I30" s="4">
         <f t="shared" si="15"/>
-        <v>0.6</v>
+        <v>0.49311629999999995</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="14"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
+        <v>0.49076999999999993</v>
+      </c>
+      <c r="M30">
+        <f>D30*gazProperties!$B$13/0.73</f>
+        <v>13934.22794308509</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="71"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="68"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="68"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="71"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B33" s="4">
         <v>0.5</v>
@@ -6195,25 +6378,33 @@
         <v>31143.3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F33" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5.2999999999999999E-2</v>
+      </c>
       <c r="H33" s="4">
         <f>C33*G33</f>
-        <v>0</v>
+        <v>2.9150000000000002E-2</v>
       </c>
       <c r="I33" s="4">
         <v>0.6</v>
       </c>
       <c r="J33" s="4">
         <f>I33-H33</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="89" t="s">
-        <v>174</v>
+        <v>0.57084999999999997</v>
+      </c>
+      <c r="M33">
+        <f>D33*gazProperties!$B$13/0.73</f>
+        <v>31287.380234828255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="60" t="s">
+        <v>173</v>
       </c>
       <c r="B34" s="4">
         <v>0.95099999999999996</v>
@@ -6226,26 +6417,34 @@
         <v>14942.59</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
       <c r="H34" s="4">
         <f t="shared" ref="H34:H38" si="17">C34*G34</f>
-        <v>0</v>
+        <v>1.35993E-2</v>
       </c>
       <c r="I34" s="4">
         <f>J33</f>
-        <v>0.6</v>
+        <v>0.57084999999999997</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" ref="J34:J38" si="18">I34-H34</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="90" t="s">
-        <v>175</v>
+        <v>0.55725069999999999</v>
+      </c>
+      <c r="M34">
+        <f>D34*gazProperties!$B$13/0.73</f>
+        <v>15011.719857020364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="61" t="s">
+        <v>174</v>
       </c>
       <c r="B35" s="4">
         <v>0.67200000000000004</v>
@@ -6258,26 +6457,34 @@
         <v>13561.03</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1.2E-2</v>
+      </c>
       <c r="H35" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>8.8704000000000005E-3</v>
       </c>
       <c r="I35" s="4">
         <f t="shared" ref="I35:I37" si="19">J34</f>
-        <v>0.6</v>
+        <v>0.55725069999999999</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="18"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="89" t="s">
-        <v>176</v>
+        <v>0.54838030000000004</v>
+      </c>
+      <c r="M35">
+        <f>D35*gazProperties!$B$13/0.73</f>
+        <v>13623.768257888953</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="60" t="s">
+        <v>175</v>
       </c>
       <c r="B36" s="4">
         <v>1.224</v>
@@ -6290,26 +6497,34 @@
         <v>11917.81</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F36" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G36" s="4">
+        <v>7.4999999999999997E-3</v>
+      </c>
       <c r="H36" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.0097999999999999E-2</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="19"/>
-        <v>0.6</v>
+        <v>0.54838030000000004</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" si="18"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="89" t="s">
-        <v>177</v>
+        <v>0.53828229999999999</v>
+      </c>
+      <c r="M36">
+        <f>D36*gazProperties!$B$13/0.73</f>
+        <v>11972.946124413229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="60" t="s">
+        <v>176</v>
       </c>
       <c r="B37" s="4">
         <v>1.42</v>
@@ -6322,26 +6537,34 @@
         <v>11047.24</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="F37" s="4">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G37" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
       <c r="H37" s="4">
         <f t="shared" ref="H37" si="20">C37*G37</f>
-        <v>0</v>
+        <v>1.0934000000000001E-2</v>
       </c>
       <c r="I37" s="4">
         <f t="shared" si="19"/>
-        <v>0.6</v>
+        <v>0.53828229999999999</v>
       </c>
       <c r="J37" s="4">
         <f t="shared" ref="J37" si="21">I37-H37</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="90" t="s">
-        <v>186</v>
+        <v>0.52734829999999999</v>
+      </c>
+      <c r="M37">
+        <f>D37*gazProperties!$B$13/0.73</f>
+        <v>11098.348550905141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="61" t="s">
+        <v>185</v>
       </c>
       <c r="B38" s="4">
         <v>0.26900000000000002</v>
@@ -6354,40 +6577,48 @@
         <v>11047.24</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F38" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.06</v>
+      </c>
       <c r="H38" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.7754000000000002E-2</v>
       </c>
       <c r="I38" s="4">
         <f>J36</f>
-        <v>0.6</v>
+        <v>0.53828229999999999</v>
       </c>
       <c r="J38" s="4">
         <f t="shared" si="18"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="68"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.52052829999999994</v>
+      </c>
+      <c r="M38">
+        <f>D38*gazProperties!$B$13/0.73</f>
+        <v>11098.348550905141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="69" t="s">
+        <v>186</v>
+      </c>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="71"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" s="4">
         <v>1.032</v>
@@ -6400,23 +6631,33 @@
         <v>1834.87</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F40" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0.08</v>
+      </c>
       <c r="H40" s="4">
         <f>C40*G40</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="4"/>
+        <v>9.0816000000000022E-2</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0.6</v>
+      </c>
       <c r="J40" s="4">
         <f>I40-H40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="89" t="s">
-        <v>188</v>
+        <v>0.50918399999999997</v>
+      </c>
+      <c r="M40">
+        <f>D40*gazProperties!$B$13/0.73</f>
+        <v>1843.3587760924281</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="B41" s="4">
         <v>0.41</v>
@@ -6431,21 +6672,32 @@
       <c r="E41" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
       <c r="H41" s="4">
         <f t="shared" ref="H41:H45" si="23">C41*G41</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="4"/>
+        <v>1.7138E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <f>J40</f>
+        <v>0.50918399999999997</v>
+      </c>
       <c r="J41" s="4">
         <f t="shared" ref="J41:J45" si="24">I41-H41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="90" t="s">
-        <v>183</v>
+        <v>0.49204599999999998</v>
+      </c>
+      <c r="M41">
+        <f>D41*gazProperties!$B$13/0.73</f>
+        <v>498.07365863036836</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="61" t="s">
+        <v>182</v>
       </c>
       <c r="B42" s="4">
         <v>7.9000000000000001E-2</v>
@@ -6458,23 +6710,34 @@
         <v>13870.06</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F42" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G42" s="4">
+        <v>2.7E-2</v>
+      </c>
       <c r="H42" s="4">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>2.3462999999999999E-3</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" ref="I42:I46" si="25">J41</f>
+        <v>0.49204599999999998</v>
+      </c>
       <c r="J42" s="4">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="89" t="s">
-        <v>186</v>
+        <v>0.48969969999999996</v>
+      </c>
+      <c r="M42">
+        <f>D42*gazProperties!$B$13/0.73</f>
+        <v>13934.22794308509</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="60" t="s">
+        <v>185</v>
       </c>
       <c r="B43" s="4">
         <v>0.26900000000000002</v>
@@ -6487,23 +6750,34 @@
         <v>11047.24</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F43" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.06</v>
+      </c>
       <c r="H43" s="4">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="4"/>
+        <v>1.7754000000000002E-2</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" si="25"/>
+        <v>0.48969969999999996</v>
+      </c>
       <c r="J43" s="4">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="90" t="s">
-        <v>189</v>
+        <v>0.47194569999999997</v>
+      </c>
+      <c r="M43">
+        <f>D43*gazProperties!$B$13/0.73</f>
+        <v>11098.348550905141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="B44" s="4">
         <v>0.29799999999999999</v>
@@ -6516,23 +6790,34 @@
         <v>870.57</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
       <c r="H44" s="4">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="4"/>
+        <v>5.9004000000000001E-3</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="25"/>
+        <v>0.47194569999999997</v>
+      </c>
       <c r="J44" s="4">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="89" t="s">
-        <v>190</v>
+        <v>0.4660453</v>
+      </c>
+      <c r="M44">
+        <f>D44*gazProperties!$B$13/0.73</f>
+        <v>874.59757350808786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="60" t="s">
+        <v>189</v>
       </c>
       <c r="B45" s="4">
         <v>7.9000000000000001E-2</v>
@@ -6545,23 +6830,34 @@
         <v>1643.22</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F45" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.05</v>
+      </c>
       <c r="H45" s="4">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="4"/>
+        <v>4.3450000000000008E-3</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="25"/>
+        <v>0.4660453</v>
+      </c>
       <c r="J45" s="4">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="89" t="s">
-        <v>173</v>
+        <v>0.46170030000000001</v>
+      </c>
+      <c r="M45">
+        <f>D45*gazProperties!$B$13/0.73</f>
+        <v>1650.8221334757231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="60" t="s">
+        <v>172</v>
       </c>
       <c r="B46" s="4">
         <v>0.56399999999999995</v>
@@ -6574,18 +6870,29 @@
         <v>1381.56</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
       <c r="H46" s="4">
-        <f t="shared" ref="H46" si="25">C46*G46</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="4"/>
+        <f t="shared" ref="H46" si="26">C46*G46</f>
+        <v>2.3575199999999998E-2</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="25"/>
+        <v>0.46170030000000001</v>
+      </c>
       <c r="J46" s="4">
-        <f t="shared" ref="J46" si="26">I46-H46</f>
-        <v>0</v>
+        <f t="shared" ref="J46" si="27">I46-H46</f>
+        <v>0.43812509999999999</v>
+      </c>
+      <c r="M46">
+        <f>D46*gazProperties!$B$13/0.73</f>
+        <v>1387.9515991314126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decorate change of autocad document
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9841008-8A44-4E37-A689-2E3583B3BE00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBAB6D6-C452-4CE0-8395-777137F40269}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -2171,21 +2171,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>8</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1.9801077682981592</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2349,13 +2349,13 @@
         <v>1.2523447967842787</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>SUM(B2:B8)</f>
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0.73337724555280348</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>36021.945</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>14.930213115639303</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>9.6366200000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>9.7037756774560009</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>10.674153245201602</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>1.0125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>2.0052387124520159</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0.2023690200000002</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>8.3802227800000022</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -2490,15 +2490,15 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="104" t="s">
         <v>150</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="105"/>
       <c r="B2" s="105"/>
       <c r="C2" s="105"/>
@@ -2576,7 +2576,7 @@
       <c r="O2" s="105"/>
       <c r="P2" s="107"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>209</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="O4" s="80"/>
       <c r="P4" s="81"/>
     </row>
-    <row r="5" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0.45</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D6:D15" si="1">B7*C7</f>
+        <f t="shared" ref="D7:D13" si="1">B7*C7</f>
         <v>1.377</v>
       </c>
       <c r="E7" s="4">
@@ -2819,7 +2819,7 @@
         <v>149.95252768369892</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>146.5021081475951</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>145.64804498602095</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>151.08776506819913</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>164.32258203214897</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>187.03022190536799</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>216.02280431033816</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>270.87540377223274</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -3234,11 +3234,11 @@
         <v>30.599999999999998</v>
       </c>
       <c r="C15" s="71">
-        <v>0.22600000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="D15" s="68">
         <f>B15*C15</f>
-        <v>6.9155999999999995</v>
+        <v>7.0686</v>
       </c>
       <c r="E15" s="69">
         <v>2.4</v>
@@ -3284,7 +3284,7 @@
         <v>311.42789666594615</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="79" t="s">
         <v>211</v>
       </c>
@@ -3304,7 +3304,7 @@
       <c r="O16" s="80"/>
       <c r="P16" s="81"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>12</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>13</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>14</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>180.6959633220101</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>15</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>177.24554378590628</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>16</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>176.39148062433213</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>17</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>181.83120070651032</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>18</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>195.06601767046016</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>19</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>217.77365754367918</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>20</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>246.76623994864934</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>21</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>298.32489987786778</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="101" t="s">
         <v>210</v>
       </c>
@@ -3903,7 +3903,7 @@
       <c r="O27" s="102"/>
       <c r="P27" s="103"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>22</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>126.24093439543113</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>23</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>153.46844885872062</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>24</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>180.6959633220101</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>177.24554378590628</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>26</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>176.39148062433213</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>27</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>181.83120070651032</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>28</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>195.06601767046016</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>29</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>217.77365754367918</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>30</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>246.76623994864934</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>31</v>
       </c>
@@ -4508,16 +4508,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976CE0B6-A4DD-4F3A-9541-7B68E6FF789C}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="104" t="s">
         <v>150</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="108"/>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -4563,7 +4563,7 @@
       <c r="I2" s="108"/>
       <c r="J2" s="109"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>222</v>
       </c>
@@ -4609,7 +4609,7 @@
       <c r="I4" s="80"/>
       <c r="J4" s="81"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="E5" s="68">
         <f>гидрРасчвнутр!D15</f>
-        <v>6.9155999999999995</v>
+        <v>7.0686</v>
       </c>
       <c r="F5" s="4">
         <v>32</v>
@@ -4647,7 +4647,7 @@
         <v>16.630484363228156</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="E6" s="4">
         <f>E5*2</f>
-        <v>13.831199999999999</v>
+        <v>14.1372</v>
       </c>
       <c r="F6" s="4">
         <v>32</v>
@@ -4681,11 +4681,11 @@
         <v>183.28122085255606</v>
       </c>
       <c r="J6" s="4">
-        <f>I6</f>
-        <v>183.28122085255606</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I6+J5</f>
+        <v>199.91170521578422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E7" s="4">
         <f>E6*2</f>
-        <v>27.662399999999998</v>
+        <v>28.2744</v>
       </c>
       <c r="F7" s="4">
         <v>50</v>
@@ -4719,11 +4719,11 @@
         <v>46.556294487237615</v>
       </c>
       <c r="J7" s="4">
-        <f>J5+I7</f>
-        <v>63.186778850465771</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <f>J6+I7</f>
+        <v>246.46799970302183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="E8" s="4">
         <f>E6*3</f>
-        <v>41.493600000000001</v>
+        <v>42.4116</v>
       </c>
       <c r="F8" s="4">
         <v>50</v>
@@ -4758,10 +4758,10 @@
       </c>
       <c r="J8" s="4">
         <f t="shared" ref="J8:J17" si="3">J7+I8</f>
-        <v>162.74424687380451</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>346.02546772636055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="E9" s="4">
         <f>E6*4</f>
-        <v>55.324799999999996</v>
+        <v>56.5488</v>
       </c>
       <c r="F9" s="4">
         <v>70</v>
@@ -4797,10 +4797,10 @@
       </c>
       <c r="J9" s="4">
         <f>J8+I9</f>
-        <v>405.1963531502883</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>588.47757400284434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="E10" s="4">
         <f>E6*10</f>
-        <v>138.31199999999998</v>
+        <v>141.37200000000001</v>
       </c>
       <c r="F10" s="4">
         <v>125</v>
@@ -4835,10 +4835,10 @@
       </c>
       <c r="J10" s="4">
         <f>J9+I10</f>
-        <v>439.9024025586782</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>623.18362341123429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="79" t="s">
         <v>223</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="I11" s="80"/>
       <c r="J11" s="81"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -4869,7 +4869,7 @@
       </c>
       <c r="E12" s="68">
         <f>гидрРасчвнутр!D15</f>
-        <v>6.9155999999999995</v>
+        <v>7.0686</v>
       </c>
       <c r="F12" s="4">
         <v>32</v>
@@ -4890,7 +4890,7 @@
         <v>18.441725234470823</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="E13" s="4">
         <f>E12*2</f>
-        <v>13.831199999999999</v>
+        <v>14.1372</v>
       </c>
       <c r="F13" s="4">
         <v>32</v>
@@ -4928,7 +4928,7 @@
         <v>156.92086987862427</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="E14" s="4">
         <f>E13+E12</f>
-        <v>20.7468</v>
+        <v>21.2058</v>
       </c>
       <c r="F14" s="4">
         <v>50</v>
@@ -4966,7 +4966,7 @@
         <v>168.2944458681481</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>9</v>
       </c>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="E15" s="4">
         <f>E13*2</f>
-        <v>27.662399999999998</v>
+        <v>28.2744</v>
       </c>
       <c r="F15" s="4">
         <v>50</v>
@@ -5000,11 +5000,11 @@
         <v>49.947812628692013</v>
       </c>
       <c r="J15" s="4">
-        <f>J12+I15</f>
-        <v>68.389537863162843</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <f>J14+I15</f>
+        <v>218.24225849684012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="E16" s="4">
         <f>E13*3</f>
-        <v>41.493600000000001</v>
+        <v>42.4116</v>
       </c>
       <c r="F16" s="4">
         <v>50</v>
@@ -5039,10 +5039,10 @@
       </c>
       <c r="J16" s="4">
         <f t="shared" si="3"/>
-        <v>156.9568957800291</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>306.80961641370641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>11</v>
       </c>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="E17" s="4">
         <f>E13*4</f>
-        <v>55.324799999999996</v>
+        <v>56.5488</v>
       </c>
       <c r="F17" s="4">
         <v>70</v>
@@ -5076,11 +5076,11 @@
         <v>41.447468039553144</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="3"/>
-        <v>198.40436381958224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <f>J16+I17</f>
+        <v>348.25708445325955</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="E18" s="4">
         <f>E13*5</f>
-        <v>69.155999999999992</v>
+        <v>70.686000000000007</v>
       </c>
       <c r="F18" s="4">
         <v>70</v>
@@ -5114,11 +5114,11 @@
         <v>64.375854614625098</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" ref="J18:J19" si="15">J17+I18</f>
-        <v>262.78021843420731</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <f>J17+I18</f>
+        <v>412.63293906788465</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>13</v>
       </c>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="E19" s="4">
         <f>E13*6</f>
-        <v>82.987200000000001</v>
+        <v>84.8232</v>
       </c>
       <c r="F19" s="4">
         <v>80</v>
@@ -5152,11 +5152,11 @@
         <v>85.439514010847205</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="15"/>
-        <v>348.21973244505455</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <f>J18+I19</f>
+        <v>498.07245307873188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5168,7 +5168,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5201,31 +5201,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879CB410-EB40-41A7-8023-5EC270239CE9}">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView topLeftCell="K8" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="16" max="16" width="25.85546875" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.88671875" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5382,7 +5382,7 @@
       <c r="T3" s="73"/>
       <c r="U3" s="75"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5421,7 +5421,7 @@
       <c r="T4" s="73"/>
       <c r="U4" s="75"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5460,7 +5460,7 @@
       <c r="T5" s="73"/>
       <c r="U5" s="75"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="T6" s="73"/>
       <c r="U6" s="75"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5538,7 +5538,7 @@
       <c r="T7" s="73"/>
       <c r="U7" s="75"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="T8" s="73"/>
       <c r="U8" s="75"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5616,7 +5616,7 @@
       <c r="T9" s="73"/>
       <c r="U9" s="75"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5655,7 +5655,7 @@
       <c r="T10" s="73"/>
       <c r="U10" s="75"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="T11" s="73"/>
       <c r="U11" s="75"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5733,7 +5733,7 @@
       <c r="T12" s="73"/>
       <c r="U12" s="75"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5772,7 +5772,7 @@
       <c r="T13" s="73"/>
       <c r="U13" s="75"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -5811,7 +5811,7 @@
       <c r="T14" s="73"/>
       <c r="U14" s="75"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5850,7 +5850,7 @@
       <c r="T15" s="73"/>
       <c r="U15" s="75"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5889,7 +5889,7 @@
       <c r="T16" s="73"/>
       <c r="U16" s="75"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -5928,7 +5928,7 @@
       <c r="T17" s="73"/>
       <c r="U17" s="75"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -5967,7 +5967,7 @@
       <c r="T18" s="73"/>
       <c r="U18" s="75"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -6006,7 +6006,7 @@
       <c r="T19" s="73"/>
       <c r="U19" s="75"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -6045,7 +6045,7 @@
       <c r="T20" s="73"/>
       <c r="U20" s="75"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -6084,7 +6084,7 @@
       <c r="T21" s="73"/>
       <c r="U21" s="75"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -6123,7 +6123,7 @@
       <c r="T22" s="73"/>
       <c r="U22" s="75"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -6162,7 +6162,7 @@
       <c r="T23" s="73"/>
       <c r="U23" s="75"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -6201,7 +6201,7 @@
       <c r="T24" s="73"/>
       <c r="U24" s="75"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6240,7 +6240,7 @@
       <c r="T25" s="73"/>
       <c r="U25" s="75"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -6279,7 +6279,7 @@
       <c r="T26" s="73"/>
       <c r="U26" s="75"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -6318,7 +6318,7 @@
       <c r="T27" s="73"/>
       <c r="U27" s="75"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -6357,7 +6357,7 @@
       <c r="T28" s="73"/>
       <c r="U28" s="75"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29">
         <f>SUM(C2:C28)</f>
         <v>234.82999999999996</v>
@@ -6423,7 +6423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J30">
         <f>SUMIF($H$2:$H$28,J2,$I$2:$I$28)</f>
         <v>6032</v>
@@ -6463,6 +6463,16 @@
       <c r="U30">
         <f t="shared" si="11"/>
         <v>5057</v>
+      </c>
+    </row>
+    <row r="33" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <f>SUM(K30:N30)</f>
+        <v>38239</v>
+      </c>
+      <c r="R33">
+        <f>SUM(R30:U30)</f>
+        <v>31757</v>
       </c>
     </row>
   </sheetData>
@@ -6490,9 +6500,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -6500,7 +6510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6508,7 +6518,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -6516,7 +6526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -6524,7 +6534,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -6532,7 +6542,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -6540,7 +6550,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -6548,7 +6558,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -6556,7 +6566,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -6564,7 +6574,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -6585,12 +6595,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -6606,7 +6616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -6624,24 +6634,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33035FD5-04D2-4D7F-99BE-F176EC4254F0}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="62" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="82" t="s">
         <v>42</v>
       </c>
@@ -6671,7 +6681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="83"/>
       <c r="B2" s="83"/>
       <c r="C2" s="83"/>
@@ -6687,7 +6697,7 @@
       <c r="I2" s="83"/>
       <c r="J2" s="83"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -6719,7 +6729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>34</v>
       </c>
@@ -6733,7 +6743,7 @@
       <c r="I4" s="77"/>
       <c r="J4" s="78"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="79" t="s">
         <v>53</v>
       </c>
@@ -6747,7 +6757,7 @@
       <c r="I5" s="80"/>
       <c r="J5" s="81"/>
     </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -6785,7 +6795,7 @@
       </c>
       <c r="L6" s="32"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="80" t="s">
         <v>56</v>
       </c>
@@ -6799,7 +6809,7 @@
       <c r="I7" s="80"/>
       <c r="J7" s="81"/>
     </row>
-    <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>2</v>
       </c>
@@ -6836,7 +6846,7 @@
         <v>1264.8223659807281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -6853,7 +6863,7 @@
         <v>1834.8767615750357</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="76" t="s">
         <v>35</v>
       </c>
@@ -6867,7 +6877,7 @@
       <c r="I10" s="77"/>
       <c r="J10" s="78"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="79" t="s">
         <v>53</v>
       </c>
@@ -6881,7 +6891,7 @@
       <c r="I11" s="80"/>
       <c r="J11" s="81"/>
     </row>
-    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>1</v>
       </c>
@@ -6918,7 +6928,7 @@
         <v>331.14565685717059</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="80" t="s">
         <v>56</v>
       </c>
@@ -6932,7 +6942,7 @@
       <c r="I13" s="80"/>
       <c r="J13" s="81"/>
     </row>
-    <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>2</v>
       </c>
@@ -6969,7 +6979,7 @@
         <v>1050.4187838711782</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -6986,7 +6996,7 @@
         <v>1381.5644407283489</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -6998,7 +7008,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -7010,7 +7020,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
@@ -7022,7 +7032,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -7034,7 +7044,7 @@
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -7046,7 +7056,7 @@
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -7058,7 +7068,7 @@
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -7097,19 +7107,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD0AAA4-CEDA-4DBB-82AC-0AD67E237AF8}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -7118,7 +7128,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -7133,12 +7143,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -7163,7 +7173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -7188,7 +7198,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E8" s="39" t="s">
         <v>31</v>
       </c>
@@ -7203,7 +7213,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" s="39" t="s">
         <v>69</v>
       </c>
@@ -7212,7 +7222,7 @@
         <v>152800</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>52&amp;"*"&amp;0.05&amp;"*"&amp;'расчетКол-ваЖит'!E29</f>
         <v>52*0.05*79532</v>
@@ -7222,7 +7232,7 @@
         <v>206783.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -7234,7 +7244,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -7243,7 +7253,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -7255,7 +7265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7267,7 +7277,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -7279,7 +7289,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -7291,7 +7301,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -7303,7 +7313,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>58</v>
       </c>
@@ -7312,12 +7322,12 @@
         <v>8426</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -7326,7 +7336,7 @@
         <v>3484</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -7335,7 +7345,7 @@
         <v>13935</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -7344,12 +7354,12 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -7370,7 +7380,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>115</v>
       </c>
@@ -7391,7 +7401,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>118</v>
       </c>
@@ -7407,7 +7417,7 @@
         <v>796878</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
@@ -7416,7 +7426,7 @@
         <v>13870.060832084442</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="E46" t="s">
         <v>114</v>
@@ -7426,7 +7436,7 @@
         <v>634698</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>111</v>
       </c>
@@ -7435,7 +7445,7 @@
         <v>67119.313500000004</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>133</v>
       </c>
@@ -7444,7 +7454,7 @@
         <v>8054.3176200000007</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>134</v>
       </c>
@@ -7453,7 +7463,7 @@
         <v>13258.136</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>135</v>
       </c>
@@ -7477,13 +7487,13 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="82" t="s">
         <v>42</v>
       </c>
@@ -7513,7 +7523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="83"/>
       <c r="B2" s="83"/>
       <c r="C2" s="83"/>
@@ -7529,7 +7539,7 @@
       <c r="I2" s="83"/>
       <c r="J2" s="83"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -7561,7 +7571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>90</v>
       </c>
@@ -7575,7 +7585,7 @@
       <c r="I4" s="77"/>
       <c r="J4" s="78"/>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>1</v>
       </c>
@@ -7612,7 +7622,7 @@
         <v>47.131763089910272</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2</v>
       </c>
@@ -7649,7 +7659,7 @@
         <v>135.50381888349202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>3</v>
       </c>
@@ -7686,7 +7696,7 @@
         <v>82.604817893552152</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>4</v>
       </c>
@@ -7708,7 +7718,7 @@
         <v>605.33020079843004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="86" t="s">
         <v>108</v>
       </c>
@@ -7727,7 +7737,7 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="91" t="s">
         <v>91</v>
       </c>
@@ -7741,7 +7751,7 @@
       <c r="I10" s="92"/>
       <c r="J10" s="93"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>1</v>
       </c>
@@ -7776,7 +7786,7 @@
         <v>40.299508165554819</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>2</v>
       </c>
@@ -7811,7 +7821,7 @@
         <v>351.38649509347704</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
         <v>3</v>
       </c>
@@ -7846,7 +7856,7 @@
         <v>104.09511017057334</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="86" t="s">
         <v>107</v>
       </c>
@@ -7865,7 +7875,7 @@
         <v>495.78111342960517</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="76" t="s">
         <v>100</v>
       </c>
@@ -7879,7 +7889,7 @@
       <c r="I15" s="77"/>
       <c r="J15" s="78"/>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="30">
         <v>1</v>
       </c>
@@ -7916,7 +7926,7 @@
         <v>85.044125596627694</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="30">
         <v>2</v>
       </c>
@@ -7953,7 +7963,7 @@
         <v>106.30515699578461</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>3</v>
       </c>
@@ -7990,7 +8000,7 @@
         <v>1451.8735827515029</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="86" t="s">
         <v>106</v>
       </c>
@@ -8009,7 +8019,7 @@
         <v>1643.2228653439151</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
@@ -8021,7 +8031,7 @@
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
@@ -8033,7 +8043,7 @@
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="B22" s="43"/>
       <c r="C22" s="43"/>
@@ -8045,7 +8055,7 @@
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -8057,7 +8067,7 @@
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
@@ -8069,7 +8079,7 @@
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
@@ -8081,7 +8091,7 @@
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="43"/>
       <c r="B26" s="43"/>
       <c r="C26" s="43"/>
@@ -8093,7 +8103,7 @@
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -8105,7 +8115,7 @@
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="43"/>
       <c r="C28" s="43"/>
@@ -8152,18 +8162,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>125</v>
       </c>
@@ -8187,7 +8197,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -8207,7 +8217,7 @@
       <c r="J2" s="43"/>
       <c r="K2" s="56"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8231,7 +8241,7 @@
       </c>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -8255,7 +8265,7 @@
         <v>870.57060066538452</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8276,7 +8286,7 @@
       <c r="I5" s="57"/>
       <c r="K5" s="58"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -8300,7 +8310,7 @@
       </c>
       <c r="K6" s="58"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8324,7 +8334,7 @@
         <v>1643.2228653439151</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -8348,7 +8358,7 @@
       </c>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8372,7 +8382,7 @@
         <v>11047.236678641313</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="95" t="s">
         <v>136</v>
       </c>
@@ -8389,7 +8399,7 @@
       <c r="I10" s="57"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -8404,7 +8414,7 @@
         <v>13561.030144650613</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -8418,7 +8428,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -8442,12 +8452,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -8459,7 +8469,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19">
         <f>B18*1000</f>
         <v>32.179198147696802</v>
@@ -8468,7 +8478,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>273</v>
       </c>
@@ -8486,13 +8496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECA6797-C0EB-4566-9FAB-3CEBA037D098}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
         <v>150</v>
       </c>
@@ -8520,7 +8530,7 @@
       </c>
       <c r="J1" s="98"/>
     </row>
-    <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="100"/>
       <c r="B2" s="59" t="s">
         <v>170</v>
@@ -8540,7 +8550,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -8572,7 +8582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>160</v>
       </c>
@@ -8586,7 +8596,7 @@
       <c r="I4" s="80"/>
       <c r="J4" s="81"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>161</v>
       </c>
@@ -8625,7 +8635,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="60" t="s">
         <v>173</v>
       </c>
@@ -8665,7 +8675,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="61" t="s">
         <v>174</v>
       </c>
@@ -8705,7 +8715,7 @@
         <v>22331.678700046548</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
         <v>175</v>
       </c>
@@ -8745,7 +8755,7 @@
         <v>21341.187429213842</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>176</v>
       </c>
@@ -8785,7 +8795,7 @@
         <v>20597.773966286964</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="60" t="s">
         <v>177</v>
       </c>
@@ -8825,7 +8835,7 @@
         <v>12274.01255310811</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="60" t="s">
         <v>178</v>
       </c>
@@ -8865,7 +8875,7 @@
         <v>1823.3466189261105</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
         <v>179</v>
       </c>
@@ -8904,7 +8914,7 @@
         <v>1474.6910393793978</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="60" t="s">
         <v>180</v>
       </c>
@@ -8944,7 +8954,7 @@
         <v>1474.6910393793978</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="79" t="s">
         <v>171</v>
       </c>
@@ -8958,7 +8968,7 @@
       <c r="I14" s="80"/>
       <c r="J14" s="81"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>161</v>
       </c>
@@ -8997,7 +9007,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="60" t="s">
         <v>162</v>
       </c>
@@ -9037,7 +9047,7 @@
         <v>23442.041988604407</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="61" t="s">
         <v>163</v>
       </c>
@@ -9077,7 +9087,7 @@
         <v>21967.350949225009</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="60" t="s">
         <v>164</v>
       </c>
@@ -9117,7 +9127,7 @@
         <v>21618.695369678295</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="61" t="s">
         <v>165</v>
       </c>
@@ -9157,7 +9167,7 @@
         <v>11168.029435496295</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
         <v>166</v>
       </c>
@@ -9197,7 +9207,7 @@
         <v>2844.2680223174393</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="60" t="s">
         <v>167</v>
       </c>
@@ -9237,7 +9247,7 @@
         <v>2100.8545593905637</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="60" t="s">
         <v>168</v>
       </c>
@@ -9277,7 +9287,7 @@
         <v>1110.3632885578575</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="60" t="s">
         <v>172</v>
       </c>
@@ -9317,7 +9327,7 @@
         <v>1110.3632885578575</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="79" t="s">
         <v>183</v>
       </c>
@@ -9331,7 +9341,7 @@
       <c r="I24" s="80"/>
       <c r="J24" s="81"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="79" t="s">
         <v>181</v>
       </c>
@@ -9345,7 +9355,7 @@
       <c r="I25" s="80"/>
       <c r="J25" s="81"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>161</v>
       </c>
@@ -9384,7 +9394,7 @@
         <v>31287.380234828255</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="60" t="s">
         <v>162</v>
       </c>
@@ -9424,7 +9434,7 @@
         <v>16275.66037780789</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="61" t="s">
         <v>163</v>
       </c>
@@ -9464,7 +9474,7 @@
         <v>14432.301601715462</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="60" t="s">
         <v>164</v>
       </c>
@@ -9504,7 +9514,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="61" t="s">
         <v>182</v>
       </c>
@@ -9544,7 +9554,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="79" t="s">
         <v>183</v>
       </c>
@@ -9558,7 +9568,7 @@
       <c r="I31" s="80"/>
       <c r="J31" s="81"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="79" t="s">
         <v>184</v>
       </c>
@@ -9572,7 +9582,7 @@
       <c r="I32" s="80"/>
       <c r="J32" s="81"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -9611,7 +9621,7 @@
         <v>31287.380234828255</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="60" t="s">
         <v>173</v>
       </c>
@@ -9651,7 +9661,7 @@
         <v>15011.719857020364</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="61" t="s">
         <v>174</v>
       </c>
@@ -9691,7 +9701,7 @@
         <v>13623.768257888953</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="60" t="s">
         <v>175</v>
       </c>
@@ -9731,7 +9741,7 @@
         <v>11972.946124413229</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="60" t="s">
         <v>176</v>
       </c>
@@ -9771,7 +9781,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="61" t="s">
         <v>185</v>
       </c>
@@ -9811,7 +9821,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="79" t="s">
         <v>186</v>
       </c>
@@ -9825,7 +9835,7 @@
       <c r="I39" s="80"/>
       <c r="J39" s="81"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>180</v>
       </c>
@@ -9864,7 +9874,7 @@
         <v>1843.3587760924281</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="60" t="s">
         <v>187</v>
       </c>
@@ -9904,7 +9914,7 @@
         <v>498.07365863036836</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="61" t="s">
         <v>182</v>
       </c>
@@ -9944,7 +9954,7 @@
         <v>13934.22794308509</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="60" t="s">
         <v>185</v>
       </c>
@@ -9984,7 +9994,7 @@
         <v>11098.348550905141</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="61" t="s">
         <v>188</v>
       </c>
@@ -10024,7 +10034,7 @@
         <v>874.59757350808786</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="60" t="s">
         <v>189</v>
       </c>
@@ -10064,7 +10074,7 @@
         <v>1650.8221334757231</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="60" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
add Aatachment B, change AttachmentA, convert lists to PDF
</commit_message>
<xml_diff>
--- a/documentation/calculation/GazProperties.xlsx
+++ b/documentation/calculation/GazProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\ASK_Diplom\documentation\calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F3B2C2-CE93-4D51-8A20-D4542B1DF452}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949BA47-406B-4E8A-A090-C77C115ED2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gazProperties" sheetId="1" r:id="rId1"/>
@@ -1777,6 +1777,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,9 +1894,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2494,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C39F77-DF6D-4F34-8291-372EBA06CCA4}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:P37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,34 +2508,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="107" t="s">
         <v>195</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="107" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="109" t="s">
         <v>198</v>
       </c>
       <c r="H1" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="104" t="s">
+      <c r="J1" s="107" t="s">
         <v>201</v>
       </c>
       <c r="K1" s="62" t="s">
@@ -2544,46 +2544,46 @@
       <c r="L1" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="104" t="s">
+      <c r="M1" s="107" t="s">
         <v>204</v>
       </c>
       <c r="N1" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="104" t="s">
+      <c r="O1" s="107" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="106" t="s">
+      <c r="P1" s="109" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
       <c r="E2" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="107"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="110"/>
       <c r="H2" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
       <c r="K2" s="63" t="s">
         <v>148</v>
       </c>
       <c r="L2" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="105"/>
+      <c r="M2" s="108"/>
       <c r="N2" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="O2" s="105"/>
-      <c r="P2" s="107"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="110"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -2636,24 +2636,24 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="81"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="84"/>
     </row>
     <row r="5" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -3191,7 +3191,7 @@
         <v>2.8447999999999998</v>
       </c>
       <c r="E14" s="4">
-        <v>11.7</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F14" s="4">
         <v>15</v>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="J14" s="4">
         <f t="shared" si="7"/>
-        <v>16.799999999999997</v>
+        <v>14.299999999999999</v>
       </c>
       <c r="K14" s="4">
         <v>3.25</v>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="M14" s="68">
         <f t="shared" si="3"/>
-        <v>54.852599461894613</v>
+        <v>46.690010256255533</v>
       </c>
       <c r="N14" s="68">
         <f>-9.81*0*(1.293-gazProperties!$B$13)</f>
@@ -3227,11 +3227,11 @@
       </c>
       <c r="O14" s="68">
         <f t="shared" si="4"/>
-        <v>54.852599461894613</v>
+        <v>46.690010256255533</v>
       </c>
       <c r="P14" s="68">
         <f t="shared" si="5"/>
-        <v>270.87540377223274</v>
+        <v>262.71281456659369</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>7.7615999999999987</v>
       </c>
       <c r="E15" s="69">
-        <v>2.4</v>
+        <v>9.6</v>
       </c>
       <c r="F15" s="69">
         <v>25</v>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="J15" s="68">
         <f t="shared" si="7"/>
-        <v>5.78</v>
+        <v>12.98</v>
       </c>
       <c r="K15" s="68">
         <v>9.82</v>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="M15" s="68">
         <f t="shared" si="3"/>
-        <v>57.02219055709439</v>
+        <v>128.0532929811566</v>
       </c>
       <c r="N15" s="68">
         <f>-9.81*3*(1.293-gazProperties!$B$13)</f>
@@ -3286,32 +3286,32 @@
       </c>
       <c r="O15" s="68">
         <f>M15+N15</f>
-        <v>40.552492893713399</v>
+        <v>111.5835953177756</v>
       </c>
       <c r="P15" s="68">
         <f>P14+O15</f>
-        <v>311.42789666594615</v>
+        <v>374.29640988436927</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="81"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="84"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -3844,12 +3844,12 @@
       <c r="C26" s="4">
         <v>0.254</v>
       </c>
-      <c r="D26" s="4">
-        <f t="shared" si="8"/>
+      <c r="D26" s="68">
+        <f>B26*C26</f>
         <v>2.8447999999999998</v>
       </c>
       <c r="E26" s="4">
-        <v>11.7</v>
+        <v>7.4</v>
       </c>
       <c r="F26" s="4">
         <v>15</v>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" si="15"/>
-        <v>16.799999999999997</v>
+        <v>12.5</v>
       </c>
       <c r="K26" s="4">
         <v>3.25</v>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="M26" s="68">
         <f t="shared" si="11"/>
-        <v>54.852599461894613</v>
+        <v>40.812946028195398</v>
       </c>
       <c r="N26" s="68">
         <f>-9.81*0.6*(1.293-gazProperties!$B$13)</f>
@@ -3885,32 +3885,32 @@
       </c>
       <c r="O26" s="68">
         <f t="shared" si="12"/>
-        <v>51.558659929218415</v>
+        <v>37.5190064955192</v>
       </c>
       <c r="P26" s="68">
         <f t="shared" si="13"/>
-        <v>298.32489987786778</v>
+        <v>284.28524644416854</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="101" t="s">
+      <c r="A27" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="102"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="102"/>
-      <c r="K27" s="102"/>
-      <c r="L27" s="102"/>
-      <c r="M27" s="102"/>
-      <c r="N27" s="102"/>
-      <c r="O27" s="102"/>
-      <c r="P27" s="103"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="105"/>
+      <c r="N27" s="105"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="106"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -4448,7 +4448,7 @@
         <v>2.8447999999999998</v>
       </c>
       <c r="E37" s="69">
-        <v>11.7</v>
+        <v>10.1</v>
       </c>
       <c r="F37" s="69">
         <v>15</v>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="J37" s="68">
         <f t="shared" si="23"/>
-        <v>16.799999999999997</v>
+        <v>15.2</v>
       </c>
       <c r="K37" s="68">
         <v>3.25</v>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="M37" s="68">
         <f t="shared" si="19"/>
-        <v>54.852599461894613</v>
+        <v>49.628542370285608</v>
       </c>
       <c r="N37" s="68">
         <f>-9.81*0*(1.293-gazProperties!$B$13)</f>
@@ -4484,11 +4484,11 @@
       </c>
       <c r="O37" s="68">
         <f t="shared" si="20"/>
-        <v>54.852599461894613</v>
+        <v>49.628542370285608</v>
       </c>
       <c r="P37" s="68">
         <f t="shared" si="21"/>
-        <v>301.61883941054396</v>
+        <v>296.39478231893497</v>
       </c>
     </row>
   </sheetData>
@@ -4515,10 +4515,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976CE0B6-A4DD-4F3A-9541-7B68E6FF789C}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,53 +4529,53 @@
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="107" t="s">
         <v>213</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="107" t="s">
         <v>216</v>
       </c>
       <c r="G1" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="107" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="107" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="106" t="s">
+      <c r="J1" s="109" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
       <c r="G2" s="63" t="s">
         <v>218</v>
       </c>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="109"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="112"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4607,34 +4607,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="82" t="s">
         <v>222</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="84"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <v>10.1</v>
+        <v>20.2</v>
       </c>
       <c r="C5" s="4">
         <f>0.1*B5</f>
-        <v>1.01</v>
+        <v>2.02</v>
       </c>
       <c r="D5" s="4">
         <f>C5+B5</f>
-        <v>11.11</v>
+        <v>22.22</v>
       </c>
       <c r="E5" s="68">
         <f>гидрРасчвнутр!D15</f>
@@ -4652,65 +4652,73 @@
       </c>
       <c r="I5" s="68">
         <f>H5*D5</f>
-        <v>16.630484363228156</v>
+        <v>33.260968726456312</v>
       </c>
       <c r="J5" s="68">
         <f>I5</f>
-        <v>16.630484363228156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+        <v>33.260968726456312</v>
+      </c>
+      <c r="L5">
+        <f>B5/2</f>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="4">
-        <v>30.6</v>
+        <v>61.2</v>
       </c>
       <c r="C6" s="4">
         <f>0.1*B6</f>
-        <v>3.0600000000000005</v>
+        <v>6.120000000000001</v>
       </c>
       <c r="D6" s="4">
         <f>C6+B6</f>
-        <v>33.660000000000004</v>
+        <v>67.320000000000007</v>
       </c>
       <c r="E6" s="68">
         <f>E5*2</f>
         <v>15.523199999999997</v>
       </c>
       <c r="F6" s="4">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G6" s="4">
-        <v>5.42</v>
+        <v>3.34</v>
       </c>
       <c r="H6" s="68">
         <f>G6*gazProperties!$B$13/0.73</f>
-        <v>5.4450748916386225</v>
+        <v>3.3554520549950189</v>
       </c>
       <c r="I6" s="68">
         <f>H6*D6</f>
-        <v>183.28122085255606</v>
+        <v>225.8890323422647</v>
       </c>
       <c r="J6" s="68">
         <f>I6+J5</f>
-        <v>199.91170521578422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>259.150001068721</v>
+      </c>
+      <c r="L6" s="65">
+        <f t="shared" ref="L6:L19" si="0">B6/2</f>
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>15.1</v>
+        <v>30.2</v>
       </c>
       <c r="C7" s="4">
         <f>0.1*B7</f>
-        <v>1.51</v>
+        <v>3.02</v>
       </c>
       <c r="D7" s="4">
         <f>C7+B7</f>
-        <v>16.61</v>
+        <v>33.22</v>
       </c>
       <c r="E7" s="68">
         <f>E6*2</f>
@@ -4728,111 +4736,122 @@
       </c>
       <c r="I7" s="68">
         <f>H7*D7</f>
-        <v>46.556294487237615</v>
+        <v>93.11258897447523</v>
       </c>
       <c r="J7" s="68">
         <f>J6+I7</f>
-        <v>246.46799970302183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>352.26259004319621</v>
+      </c>
+      <c r="L7" s="65">
+        <f t="shared" si="0"/>
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="4">
-        <v>15.4</v>
+        <v>30.8</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:C17" si="0">0.1*B8</f>
-        <v>1.54</v>
+        <f t="shared" ref="C8:C17" si="1">0.1*B8</f>
+        <v>3.08</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" ref="D8:D17" si="1">C8+B8</f>
-        <v>16.940000000000001</v>
+        <f t="shared" ref="D8:D17" si="2">C8+B8</f>
+        <v>33.880000000000003</v>
       </c>
       <c r="E8" s="68">
         <f>E6*3</f>
         <v>46.569599999999994</v>
       </c>
       <c r="F8" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G8" s="4">
-        <v>5.85</v>
+        <v>2.12</v>
       </c>
       <c r="H8" s="68">
         <f>G8*gazProperties!$B$13/0.73</f>
-        <v>5.8770642280601368</v>
+        <v>2.1298078911944431</v>
       </c>
       <c r="I8" s="68">
-        <f t="shared" ref="I8:I17" si="2">H8*D8</f>
-        <v>99.557468023338728</v>
+        <f t="shared" ref="I8:I17" si="3">H8*D8</f>
+        <v>72.157891353667736</v>
       </c>
       <c r="J8" s="68">
-        <f t="shared" ref="J8:J16" si="3">J7+I8</f>
-        <v>346.02546772636055</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J8:J16" si="4">J7+I8</f>
+        <v>424.42048139686392</v>
+      </c>
+      <c r="L8" s="65">
+        <f t="shared" si="0"/>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="4">
-        <f>12.6+65.2</f>
-        <v>77.8</v>
+        <v>155.6</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>7.78</v>
+        <f t="shared" si="1"/>
+        <v>15.56</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="1"/>
-        <v>85.58</v>
+        <f t="shared" si="2"/>
+        <v>171.16</v>
       </c>
       <c r="E9" s="68">
         <f>E6*4</f>
         <v>62.09279999999999</v>
       </c>
       <c r="F9" s="4">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4">
-        <v>2.82</v>
+        <v>1.49</v>
       </c>
       <c r="H9" s="68">
         <f>G9*gazProperties!$B$13/0.73</f>
-        <v>2.8330463458341177</v>
+        <v>1.4968932820187359</v>
       </c>
       <c r="I9" s="68">
         <f>H9*D9</f>
-        <v>242.45210627648379</v>
+        <v>256.20825415032687</v>
       </c>
       <c r="J9" s="68">
         <f>J8+I9</f>
-        <v>588.47757400284434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>680.62873554719079</v>
+      </c>
+      <c r="L9" s="65">
+        <f t="shared" si="0"/>
+        <v>77.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
       <c r="B10" s="4">
-        <v>36.14</v>
+        <v>72.28</v>
       </c>
       <c r="C10" s="68">
-        <f t="shared" si="0"/>
-        <v>3.6140000000000003</v>
+        <f t="shared" si="1"/>
+        <v>7.2280000000000006</v>
       </c>
       <c r="D10" s="68">
-        <f t="shared" si="1"/>
-        <v>39.753999999999998</v>
+        <f t="shared" si="2"/>
+        <v>79.507999999999996</v>
       </c>
       <c r="E10" s="68">
         <f>E6*10</f>
         <v>155.23199999999997</v>
       </c>
       <c r="F10" s="4">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="G10" s="4">
         <v>3.16</v>
@@ -4842,42 +4861,47 @@
         <v>3.1746193095162458</v>
       </c>
       <c r="I10" s="68">
-        <f t="shared" si="2"/>
-        <v>126.20381603050883</v>
+        <f t="shared" si="3"/>
+        <v>252.40763206101767</v>
       </c>
       <c r="J10" s="68">
         <f>J9+I10</f>
-        <v>714.68139003335318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+        <v>933.03636760820848</v>
+      </c>
+      <c r="L10" s="65">
+        <f t="shared" si="0"/>
+        <v>36.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="82" t="s">
         <v>223</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="84"/>
+      <c r="L11" s="65"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>7</v>
       </c>
       <c r="B12" s="4">
-        <v>11.2</v>
+        <v>22.4</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1199999999999999</v>
+        <f t="shared" si="1"/>
+        <v>2.2399999999999998</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="1"/>
-        <v>12.319999999999999</v>
+        <f t="shared" si="2"/>
+        <v>24.639999999999997</v>
       </c>
       <c r="E12" s="68">
         <f>гидрРасчвнутр!D15</f>
@@ -4894,66 +4918,74 @@
         <v>1.4968932820187359</v>
       </c>
       <c r="I12" s="68">
-        <f t="shared" si="2"/>
-        <v>18.441725234470823</v>
+        <f t="shared" si="3"/>
+        <v>36.883450468941646</v>
       </c>
       <c r="J12" s="68">
-        <f t="shared" si="3"/>
-        <v>18.441725234470823</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>36.883450468941646</v>
+      </c>
+      <c r="L12" s="65">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>8</v>
       </c>
       <c r="B13" s="4">
-        <v>23.12</v>
+        <v>46.24</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" ref="C13" si="4">0.1*B13</f>
-        <v>2.3120000000000003</v>
+        <f t="shared" ref="C13" si="5">0.1*B13</f>
+        <v>4.6240000000000006</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13" si="5">C13+B13</f>
-        <v>25.432000000000002</v>
+        <f t="shared" ref="D13" si="6">C13+B13</f>
+        <v>50.864000000000004</v>
       </c>
       <c r="E13" s="68">
         <f>E12*2</f>
         <v>15.523199999999997</v>
       </c>
       <c r="F13" s="4">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G13" s="4">
-        <v>5.42</v>
+        <v>3.34</v>
       </c>
       <c r="H13" s="68">
         <f>G13*gazProperties!$B$13/0.73</f>
-        <v>5.4450748916386225</v>
+        <v>3.3554520549950189</v>
       </c>
       <c r="I13" s="68">
-        <f t="shared" ref="I13" si="6">H13*D13</f>
-        <v>138.47914464415345</v>
+        <f t="shared" ref="I13" si="7">H13*D13</f>
+        <v>170.67171332526667</v>
       </c>
       <c r="J13" s="68">
-        <f t="shared" ref="J13" si="7">J12+I13</f>
-        <v>156.92086987862427</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J13" si="8">J12+I13</f>
+        <v>207.55516379420831</v>
+      </c>
+      <c r="L13" s="65">
+        <f t="shared" si="0"/>
+        <v>23.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
       <c r="B14" s="4">
-        <v>6.2</v>
+        <v>12.4</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14" si="8">0.1*B14</f>
-        <v>0.62000000000000011</v>
+        <f t="shared" ref="C14" si="9">0.1*B14</f>
+        <v>1.2400000000000002</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" ref="D14" si="9">C14+B14</f>
-        <v>6.82</v>
+        <f t="shared" ref="D14" si="10">C14+B14</f>
+        <v>13.64</v>
       </c>
       <c r="E14" s="68">
         <f>E13+E12</f>
@@ -4970,28 +5002,32 @@
         <v>1.6676797638597998</v>
       </c>
       <c r="I14" s="68">
-        <f t="shared" ref="I14" si="10">H14*D14</f>
-        <v>11.373575989523834</v>
+        <f t="shared" ref="I14" si="11">H14*D14</f>
+        <v>22.747151979047668</v>
       </c>
       <c r="J14" s="68">
-        <f t="shared" ref="J14" si="11">J13+I14</f>
-        <v>168.2944458681481</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J14" si="12">J13+I14</f>
+        <v>230.30231577325597</v>
+      </c>
+      <c r="L14" s="65">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>9</v>
       </c>
       <c r="B15" s="4">
-        <v>16.2</v>
+        <v>32.4</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="0"/>
-        <v>1.62</v>
+        <f t="shared" si="1"/>
+        <v>3.24</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
-        <v>17.82</v>
+        <f t="shared" si="2"/>
+        <v>35.64</v>
       </c>
       <c r="E15" s="68">
         <f>E13*2</f>
@@ -5008,142 +5044,158 @@
         <v>2.8029075549209885</v>
       </c>
       <c r="I15" s="68">
-        <f t="shared" si="2"/>
-        <v>49.947812628692013</v>
+        <f t="shared" si="3"/>
+        <v>99.895625257384026</v>
       </c>
       <c r="J15" s="68">
         <f>J14+I15</f>
-        <v>218.24225849684012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>330.19794103063998</v>
+      </c>
+      <c r="L15" s="65">
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>10</v>
       </c>
       <c r="B16" s="4">
-        <v>13.7</v>
+        <v>27.4</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="0"/>
-        <v>1.37</v>
+        <f t="shared" si="1"/>
+        <v>2.74</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>15.07</v>
+        <f t="shared" si="2"/>
+        <v>30.14</v>
       </c>
       <c r="E16" s="68">
         <f>E13*3</f>
         <v>46.569599999999994</v>
       </c>
       <c r="F16" s="4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G16" s="4">
-        <v>5.85</v>
+        <v>2.12</v>
       </c>
       <c r="H16" s="68">
         <f>G16*gazProperties!$B$13/0.73</f>
-        <v>5.8770642280601368</v>
+        <v>2.1298078911944431</v>
       </c>
       <c r="I16" s="68">
-        <f t="shared" si="2"/>
-        <v>88.567357916866257</v>
+        <f t="shared" si="3"/>
+        <v>64.192409840600519</v>
       </c>
       <c r="J16" s="68">
-        <f t="shared" si="3"/>
-        <v>306.80961641370641</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>394.39035087124051</v>
+      </c>
+      <c r="L16" s="65">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>11</v>
       </c>
       <c r="B17" s="4">
-        <v>13.3</v>
+        <v>26.6</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="0"/>
-        <v>1.33</v>
+        <f t="shared" si="1"/>
+        <v>2.66</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
-        <v>14.63</v>
+        <f t="shared" si="2"/>
+        <v>29.26</v>
       </c>
       <c r="E17" s="68">
         <f>E13*4</f>
         <v>62.09279999999999</v>
       </c>
       <c r="F17" s="4">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G17" s="4">
-        <v>2.82</v>
+        <v>1.49</v>
       </c>
       <c r="H17" s="68">
         <f>G17*gazProperties!$B$13/0.73</f>
-        <v>2.8330463458341177</v>
+        <v>1.4968932820187359</v>
       </c>
       <c r="I17" s="68">
-        <f t="shared" si="2"/>
-        <v>41.447468039553144</v>
+        <f t="shared" si="3"/>
+        <v>43.799097431868219</v>
       </c>
       <c r="J17" s="68">
         <f>J16+I17</f>
-        <v>348.25708445325955</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>438.18944830310875</v>
+      </c>
+      <c r="L17" s="65">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>12</v>
       </c>
       <c r="B18" s="4">
-        <v>13.3</v>
+        <v>26.6</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" ref="C18:C19" si="12">0.1*B18</f>
-        <v>1.33</v>
+        <f t="shared" ref="C18:C19" si="13">0.1*B18</f>
+        <v>2.66</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" ref="D18:D19" si="13">C18+B18</f>
-        <v>14.63</v>
+        <f t="shared" ref="D18:D19" si="14">C18+B18</f>
+        <v>29.26</v>
       </c>
       <c r="E18" s="68">
         <f>E13*5</f>
         <v>77.615999999999985</v>
       </c>
       <c r="F18" s="4">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G18" s="4">
-        <v>4.38</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="H18" s="68">
         <f>G18*gazProperties!$B$13/0.73</f>
-        <v>4.4002634733168211</v>
+        <v>2.2704555821223775</v>
       </c>
       <c r="I18" s="68">
-        <f t="shared" ref="I18:I19" si="14">H18*D18</f>
-        <v>64.375854614625098</v>
+        <f t="shared" ref="I18:I19" si="15">H18*D18</f>
+        <v>66.433530332900773</v>
       </c>
       <c r="J18" s="68">
         <f>J17+I18</f>
-        <v>412.63293906788465</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>504.62297863600952</v>
+      </c>
+      <c r="L18" s="65">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>13</v>
       </c>
       <c r="B19" s="4">
-        <v>31.1</v>
+        <v>62.2</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="12"/>
-        <v>3.1100000000000003</v>
+        <f t="shared" si="13"/>
+        <v>6.2200000000000006</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="13"/>
-        <v>34.21</v>
+        <f t="shared" si="14"/>
+        <v>68.42</v>
       </c>
       <c r="E19" s="68">
         <f>E13*6</f>
@@ -5160,15 +5212,19 @@
         <v>2.4975011403346157</v>
       </c>
       <c r="I19" s="68">
-        <f t="shared" si="14"/>
-        <v>85.439514010847205</v>
+        <f t="shared" si="15"/>
+        <v>170.87902802169441</v>
       </c>
       <c r="J19" s="68">
         <f>J18+I19</f>
-        <v>498.07245307873188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>675.50200665770399</v>
+      </c>
+      <c r="L19" s="65">
+        <f t="shared" si="0"/>
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5180,7 +5236,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -5322,36 +5378,36 @@
         <f>E2</f>
         <v>897</v>
       </c>
-      <c r="J2" s="72">
+      <c r="J2" s="75">
         <v>5</v>
       </c>
-      <c r="K2" s="72">
+      <c r="K2" s="75">
         <v>6</v>
       </c>
-      <c r="L2" s="72">
+      <c r="L2" s="75">
         <v>7</v>
       </c>
-      <c r="M2" s="72">
+      <c r="M2" s="75">
         <v>8</v>
       </c>
-      <c r="N2" s="74">
+      <c r="N2" s="77">
         <v>9</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="72">
+      <c r="Q2" s="75">
         <v>5</v>
       </c>
-      <c r="R2" s="72">
+      <c r="R2" s="75">
         <v>6</v>
       </c>
-      <c r="S2" s="72">
+      <c r="S2" s="75">
         <v>7</v>
       </c>
-      <c r="T2" s="72">
+      <c r="T2" s="75">
         <v>8</v>
       </c>
-      <c r="U2" s="74">
+      <c r="U2" s="77">
         <v>9</v>
       </c>
     </row>
@@ -5381,18 +5437,18 @@
         <f t="shared" ref="I3:I28" si="2">E3</f>
         <v>1670</v>
       </c>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="75"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="78"/>
       <c r="O3" s="11"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="75"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="78"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -5420,18 +5476,18 @@
         <f t="shared" si="2"/>
         <v>1899</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="75"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="78"/>
       <c r="O4" s="11"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="75"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="78"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -5459,18 +5515,18 @@
         <f t="shared" si="2"/>
         <v>3707</v>
       </c>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="78"/>
       <c r="O5" s="11"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="75"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="78"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -5498,18 +5554,18 @@
         <f t="shared" si="2"/>
         <v>5032</v>
       </c>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="75"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="78"/>
       <c r="O6" s="11"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
-      <c r="T6" s="73"/>
-      <c r="U6" s="75"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="78"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -5531,11 +5587,11 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="75"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="78"/>
       <c r="O7" s="25">
         <f>B7</f>
         <v>7</v>
@@ -5544,11 +5600,11 @@
         <f t="shared" ref="P7:P12" si="3">E7</f>
         <v>5824</v>
       </c>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
-      <c r="U7" s="75"/>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="78"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -5570,11 +5626,11 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="75"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="78"/>
       <c r="O8" s="25">
         <f t="shared" ref="O8:O12" si="4">B8</f>
         <v>8</v>
@@ -5583,11 +5639,11 @@
         <f t="shared" si="3"/>
         <v>2793</v>
       </c>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="75"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="78"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -5609,11 +5665,11 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="75"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="78"/>
       <c r="O9" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -5622,11 +5678,11 @@
         <f t="shared" si="3"/>
         <v>3476</v>
       </c>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="75"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="76"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="78"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -5648,11 +5704,11 @@
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="75"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="78"/>
       <c r="O10" s="25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -5661,11 +5717,11 @@
         <f t="shared" si="3"/>
         <v>1348</v>
       </c>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="75"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="78"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -5687,11 +5743,11 @@
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="78"/>
       <c r="O11" s="25">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -5700,11 +5756,11 @@
         <f t="shared" si="3"/>
         <v>4547</v>
       </c>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="75"/>
+      <c r="Q11" s="76"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="76"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="78"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -5726,11 +5782,11 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="75"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="78"/>
       <c r="O12" s="25">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -5739,11 +5795,11 @@
         <f t="shared" si="3"/>
         <v>2048</v>
       </c>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
-      <c r="S12" s="73"/>
-      <c r="T12" s="73"/>
-      <c r="U12" s="75"/>
+      <c r="Q12" s="76"/>
+      <c r="R12" s="76"/>
+      <c r="S12" s="76"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="78"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -5771,18 +5827,18 @@
         <f t="shared" si="2"/>
         <v>3178</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="75"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="78"/>
       <c r="O13" s="11"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="73"/>
-      <c r="U13" s="75"/>
+      <c r="Q13" s="76"/>
+      <c r="R13" s="76"/>
+      <c r="S13" s="76"/>
+      <c r="T13" s="76"/>
+      <c r="U13" s="78"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -5810,18 +5866,18 @@
         <f t="shared" si="2"/>
         <v>1806</v>
       </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="75"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="78"/>
       <c r="O14" s="11"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
-      <c r="S14" s="73"/>
-      <c r="T14" s="73"/>
-      <c r="U14" s="75"/>
+      <c r="Q14" s="76"/>
+      <c r="R14" s="76"/>
+      <c r="S14" s="76"/>
+      <c r="T14" s="76"/>
+      <c r="U14" s="78"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -5849,18 +5905,18 @@
         <f t="shared" si="2"/>
         <v>1853</v>
       </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="75"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="78"/>
       <c r="O15" s="11"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="75"/>
+      <c r="Q15" s="76"/>
+      <c r="R15" s="76"/>
+      <c r="S15" s="76"/>
+      <c r="T15" s="76"/>
+      <c r="U15" s="78"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -5888,18 +5944,18 @@
         <f t="shared" si="2"/>
         <v>1057</v>
       </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="75"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="78"/>
       <c r="O16" s="11"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="75"/>
+      <c r="Q16" s="76"/>
+      <c r="R16" s="76"/>
+      <c r="S16" s="76"/>
+      <c r="T16" s="76"/>
+      <c r="U16" s="78"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -5927,18 +5983,18 @@
         <f t="shared" si="2"/>
         <v>1757</v>
       </c>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="75"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="78"/>
       <c r="O17" s="11"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
-      <c r="S17" s="73"/>
-      <c r="T17" s="73"/>
-      <c r="U17" s="75"/>
+      <c r="Q17" s="76"/>
+      <c r="R17" s="76"/>
+      <c r="S17" s="76"/>
+      <c r="T17" s="76"/>
+      <c r="U17" s="78"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -5966,18 +6022,18 @@
         <f t="shared" si="2"/>
         <v>2128</v>
       </c>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="75"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="78"/>
       <c r="O18" s="11"/>
       <c r="P18" s="4"/>
-      <c r="Q18" s="73"/>
-      <c r="R18" s="73"/>
-      <c r="S18" s="73"/>
-      <c r="T18" s="73"/>
-      <c r="U18" s="75"/>
+      <c r="Q18" s="76"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
+      <c r="T18" s="76"/>
+      <c r="U18" s="78"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -6005,18 +6061,18 @@
         <f t="shared" si="2"/>
         <v>4505</v>
       </c>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="75"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="78"/>
       <c r="O19" s="11"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="73"/>
-      <c r="T19" s="73"/>
-      <c r="U19" s="75"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="76"/>
+      <c r="S19" s="76"/>
+      <c r="T19" s="76"/>
+      <c r="U19" s="78"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -6044,18 +6100,18 @@
         <f t="shared" si="2"/>
         <v>3329</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="75"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="78"/>
       <c r="O20" s="11"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="73"/>
-      <c r="R20" s="73"/>
-      <c r="S20" s="73"/>
-      <c r="T20" s="73"/>
-      <c r="U20" s="75"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="78"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -6077,11 +6133,11 @@
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="75"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="78"/>
       <c r="O21" s="25">
         <f>B21</f>
         <v>5</v>
@@ -6090,11 +6146,11 @@
         <f>E21</f>
         <v>2156</v>
       </c>
-      <c r="Q21" s="73"/>
-      <c r="R21" s="73"/>
-      <c r="S21" s="73"/>
-      <c r="T21" s="73"/>
-      <c r="U21" s="75"/>
+      <c r="Q21" s="76"/>
+      <c r="R21" s="76"/>
+      <c r="S21" s="76"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="78"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -6116,11 +6172,11 @@
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="75"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="78"/>
       <c r="O22" s="25">
         <f t="shared" ref="O22:O25" si="6">B22</f>
         <v>8</v>
@@ -6129,11 +6185,11 @@
         <f>E22</f>
         <v>1645</v>
       </c>
-      <c r="Q22" s="73"/>
-      <c r="R22" s="73"/>
-      <c r="S22" s="73"/>
-      <c r="T22" s="73"/>
-      <c r="U22" s="75"/>
+      <c r="Q22" s="76"/>
+      <c r="R22" s="76"/>
+      <c r="S22" s="76"/>
+      <c r="T22" s="76"/>
+      <c r="U22" s="78"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -6155,11 +6211,11 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="75"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="78"/>
       <c r="O23" s="25">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -6168,11 +6224,11 @@
         <f>E23</f>
         <v>1551</v>
       </c>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
-      <c r="S23" s="73"/>
-      <c r="T23" s="73"/>
-      <c r="U23" s="75"/>
+      <c r="Q23" s="76"/>
+      <c r="R23" s="76"/>
+      <c r="S23" s="76"/>
+      <c r="T23" s="76"/>
+      <c r="U23" s="78"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -6194,11 +6250,11 @@
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="75"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="78"/>
       <c r="O24" s="25">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -6207,11 +6263,11 @@
         <f>E24</f>
         <v>4816</v>
       </c>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="73"/>
-      <c r="S24" s="73"/>
-      <c r="T24" s="73"/>
-      <c r="U24" s="75"/>
+      <c r="Q24" s="76"/>
+      <c r="R24" s="76"/>
+      <c r="S24" s="76"/>
+      <c r="T24" s="76"/>
+      <c r="U24" s="78"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -6233,11 +6289,11 @@
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="75"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="78"/>
       <c r="O25" s="25">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -6246,11 +6302,11 @@
         <f>E25</f>
         <v>5057</v>
       </c>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="73"/>
-      <c r="S25" s="73"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="75"/>
+      <c r="Q25" s="76"/>
+      <c r="R25" s="76"/>
+      <c r="S25" s="76"/>
+      <c r="T25" s="76"/>
+      <c r="U25" s="78"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -6278,18 +6334,18 @@
         <f t="shared" si="2"/>
         <v>4484</v>
       </c>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="75"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="78"/>
       <c r="O26" s="11"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="73"/>
-      <c r="S26" s="73"/>
-      <c r="T26" s="73"/>
-      <c r="U26" s="75"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="76"/>
+      <c r="S26" s="76"/>
+      <c r="T26" s="76"/>
+      <c r="U26" s="78"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -6317,18 +6373,18 @@
         <f t="shared" si="2"/>
         <v>3486</v>
       </c>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="75"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="78"/>
       <c r="O27" s="11"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="73"/>
-      <c r="S27" s="73"/>
-      <c r="T27" s="73"/>
-      <c r="U27" s="75"/>
+      <c r="Q27" s="76"/>
+      <c r="R27" s="76"/>
+      <c r="S27" s="76"/>
+      <c r="T27" s="76"/>
+      <c r="U27" s="78"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
@@ -6356,18 +6412,18 @@
         <f t="shared" si="2"/>
         <v>3483</v>
       </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="75"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="78"/>
       <c r="O28" s="17"/>
       <c r="P28" s="16"/>
-      <c r="Q28" s="73"/>
-      <c r="R28" s="73"/>
-      <c r="S28" s="73"/>
-      <c r="T28" s="73"/>
-      <c r="U28" s="75"/>
+      <c r="Q28" s="76"/>
+      <c r="R28" s="76"/>
+      <c r="S28" s="76"/>
+      <c r="T28" s="76"/>
+      <c r="U28" s="78"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29">
@@ -6665,50 +6721,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="88"/>
+      <c r="H1" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="82" t="s">
+      <c r="I1" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="82" t="s">
+      <c r="J1" s="85" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -6743,32 +6799,32 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="84"/>
     </row>
     <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
@@ -6809,18 +6865,18 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="84"/>
     </row>
     <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
@@ -6877,32 +6933,32 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="78"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="81"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
@@ -6942,18 +6998,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="84"/>
     </row>
     <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
@@ -7532,50 +7588,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="88"/>
+      <c r="H1" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="82" t="s">
+      <c r="I1" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="82" t="s">
+      <c r="J1" s="85" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
@@ -7610,18 +7666,18 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
@@ -7741,32 +7797,32 @@
       <c r="B8" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="88" t="str">
+      <c r="C8" s="91" t="str">
         <f>РасхСосредоточПотреб!C6&amp;"+"&amp;РасхСосредоточПотреб!C7</f>
         <v>376.27+229.06</v>
       </c>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="93"/>
       <c r="J8" s="30">
         <f>РасхСосредоточПотреб!B6+РасхСосредоточПотреб!B7</f>
         <v>605.33020079843004</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="87"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
       <c r="I9" s="41" t="s">
         <v>58</v>
       </c>
@@ -7776,18 +7832,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="93"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="96"/>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
@@ -7796,10 +7852,10 @@
       <c r="B11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="90"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="30">
         <f>РасхСосредоточПотреб!B31</f>
         <v>3484</v>
@@ -7831,10 +7887,10 @@
       <c r="B12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="94" t="s">
+      <c r="C12" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="90"/>
+      <c r="D12" s="93"/>
       <c r="E12" s="30">
         <f>РасхСосредоточПотреб!B32</f>
         <v>13935</v>
@@ -7866,10 +7922,10 @@
       <c r="B13" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="90"/>
+      <c r="D13" s="93"/>
       <c r="E13" s="30">
         <f>РасхСосредоточПотреб!B33</f>
         <v>2903</v>
@@ -7895,16 +7951,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="87"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="90"/>
       <c r="I14" s="42" t="s">
         <v>58</v>
       </c>
@@ -7914,18 +7970,18 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="78"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="81"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
@@ -8039,16 +8095,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="87"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="90"/>
       <c r="I19" s="41" t="s">
         <v>58</v>
       </c>
@@ -8175,6 +8231,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -8185,15 +8250,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8278,7 +8334,7 @@
       <c r="D3" s="5">
         <v>0.8</v>
       </c>
-      <c r="E3" s="112">
+      <c r="E3" s="74">
         <f>C3*D3</f>
         <v>1467.9014092600287</v>
       </c>
@@ -8302,7 +8358,7 @@
       <c r="D4" s="4">
         <v>0.8</v>
       </c>
-      <c r="E4" s="112">
+      <c r="E4" s="74">
         <f t="shared" ref="E4:E9" si="0">C4*D4</f>
         <v>1105.2515525826791</v>
       </c>
@@ -8326,7 +8382,7 @@
       <c r="D5" s="4">
         <v>0.85</v>
       </c>
-      <c r="E5" s="112">
+      <c r="E5" s="74">
         <f t="shared" si="0"/>
         <v>739.98501056557677</v>
       </c>
@@ -8350,7 +8406,7 @@
       <c r="D6" s="4">
         <v>0.7</v>
       </c>
-      <c r="E6" s="112">
+      <c r="E6" s="74">
         <f t="shared" si="0"/>
         <v>347.04677940072361</v>
       </c>
@@ -8374,7 +8430,7 @@
       <c r="D7" s="4">
         <v>0.6</v>
       </c>
-      <c r="E7" s="112">
+      <c r="E7" s="74">
         <f t="shared" si="0"/>
         <v>984.27955514339919</v>
       </c>
@@ -8398,7 +8454,7 @@
       <c r="D8" s="4">
         <v>0.75</v>
       </c>
-      <c r="E8" s="112">
+      <c r="E8" s="74">
         <f t="shared" si="0"/>
         <v>10402.545624063332</v>
       </c>
@@ -8422,7 +8478,7 @@
       <c r="D9" s="4">
         <v>0.75</v>
       </c>
-      <c r="E9" s="112">
+      <c r="E9" s="74">
         <f t="shared" si="0"/>
         <v>8285.4275089809853</v>
       </c>
@@ -8433,10 +8489,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="98" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="96"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="4">
         <f>SUM(C3:C9)</f>
         <v>31140.556352363128</v>
@@ -8546,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECA6797-C0EB-4566-9FAB-3CEBA037D098}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J46" sqref="A40:J46"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8557,46 +8613,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="99" t="s">
+      <c r="C1" s="101"/>
+      <c r="D1" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="102" t="s">
         <v>155</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="97" t="s">
+      <c r="I1" s="100" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="98"/>
+      <c r="J1" s="101"/>
     </row>
     <row r="2" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
+      <c r="A2" s="103"/>
       <c r="B2" s="59" t="s">
         <v>170</v>
       </c>
       <c r="C2" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
       <c r="I2" s="59" t="s">
         <v>157</v>
       </c>
@@ -8637,18 +8693,18 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="84"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -8673,14 +8729,14 @@
       <c r="G5" s="4">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H5" s="110">
+      <c r="H5" s="72">
         <f>C5*G5</f>
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="I5" s="110">
+      <c r="I5" s="72">
         <v>0.6</v>
       </c>
-      <c r="J5" s="111">
+      <c r="J5" s="73">
         <f>I5-H5</f>
         <v>0.58019999999999994</v>
       </c>
@@ -8712,15 +8768,15 @@
       <c r="G6" s="4">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H6" s="110">
+      <c r="H6" s="72">
         <f t="shared" ref="H6:H10" si="1">C6*G6</f>
         <v>3.7659600000000001E-2</v>
       </c>
-      <c r="I6" s="110">
+      <c r="I6" s="72">
         <f>J5</f>
         <v>0.58019999999999994</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="73">
         <f t="shared" ref="J6:J10" si="2">I6-H6</f>
         <v>0.54254039999999992</v>
       </c>
@@ -8752,15 +8808,15 @@
       <c r="G7" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="H7" s="110">
+      <c r="H7" s="72">
         <f t="shared" si="1"/>
         <v>2.5872000000000006E-2</v>
       </c>
-      <c r="I7" s="110">
+      <c r="I7" s="72">
         <f t="shared" ref="I7:I13" si="3">J6</f>
         <v>0.54254039999999992</v>
       </c>
-      <c r="J7" s="111">
+      <c r="J7" s="73">
         <f t="shared" si="2"/>
         <v>0.51666839999999992</v>
       </c>
@@ -8792,15 +8848,15 @@
       <c r="G8" s="4">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="H8" s="110">
+      <c r="H8" s="72">
         <f t="shared" si="1"/>
         <v>4.5777600000000002E-2</v>
       </c>
-      <c r="I8" s="110">
+      <c r="I8" s="72">
         <f t="shared" si="3"/>
         <v>0.51666839999999992</v>
       </c>
-      <c r="J8" s="111">
+      <c r="J8" s="73">
         <f t="shared" si="2"/>
         <v>0.47089079999999994</v>
       </c>
@@ -8832,15 +8888,15 @@
       <c r="G9" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H9" s="110">
+      <c r="H9" s="72">
         <f t="shared" si="1"/>
         <v>5.1546000000000002E-2</v>
       </c>
-      <c r="I9" s="110">
+      <c r="I9" s="72">
         <f t="shared" si="3"/>
         <v>0.47089079999999994</v>
       </c>
-      <c r="J9" s="111">
+      <c r="J9" s="73">
         <f t="shared" si="2"/>
         <v>0.41934479999999996</v>
       </c>
@@ -8872,15 +8928,15 @@
       <c r="G10" s="4">
         <v>8.6E-3</v>
       </c>
-      <c r="H10" s="110">
+      <c r="H10" s="72">
         <f t="shared" si="1"/>
         <v>1.3045340000000001E-2</v>
       </c>
-      <c r="I10" s="110">
+      <c r="I10" s="72">
         <f t="shared" si="3"/>
         <v>0.41934479999999996</v>
       </c>
-      <c r="J10" s="111">
+      <c r="J10" s="73">
         <f t="shared" si="2"/>
         <v>0.40629945999999995</v>
       </c>
@@ -8912,15 +8968,15 @@
       <c r="G11" s="4">
         <v>2.41E-4</v>
       </c>
-      <c r="H11" s="110">
+      <c r="H11" s="72">
         <f t="shared" ref="H11:H13" si="4">C11*G11</f>
         <v>5.4265970000000015E-4</v>
       </c>
-      <c r="I11" s="110">
+      <c r="I11" s="72">
         <f t="shared" si="3"/>
         <v>0.40629945999999995</v>
       </c>
-      <c r="J11" s="111">
+      <c r="J11" s="73">
         <f t="shared" ref="J11:J13" si="5">I11-H11</f>
         <v>0.40575680029999994</v>
       </c>
@@ -8952,14 +9008,14 @@
       <c r="G12" s="4">
         <v>2.2599999999999999E-4</v>
       </c>
-      <c r="H12" s="110">
+      <c r="H12" s="72">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="I12" s="110">
+      <c r="I12" s="72">
         <f t="shared" si="3"/>
         <v>0.40575680029999994</v>
       </c>
-      <c r="J12" s="111">
+      <c r="J12" s="73">
         <f t="shared" si="5"/>
         <v>0.40551680029999992</v>
       </c>
@@ -8991,15 +9047,15 @@
       <c r="G13" s="4">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H13" s="110">
+      <c r="H13" s="72">
         <f t="shared" si="4"/>
         <v>4.8813600000000006E-2</v>
       </c>
-      <c r="I13" s="110">
+      <c r="I13" s="72">
         <f t="shared" si="3"/>
         <v>0.40551680029999992</v>
       </c>
-      <c r="J13" s="111">
+      <c r="J13" s="73">
         <f t="shared" si="5"/>
         <v>0.35670320029999991</v>
       </c>
@@ -9009,18 +9065,18 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="84"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -9045,14 +9101,14 @@
       <c r="G15" s="4">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H15" s="110">
+      <c r="H15" s="72">
         <f>C15*G15</f>
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="I15" s="111">
+      <c r="I15" s="73">
         <v>0.6</v>
       </c>
-      <c r="J15" s="111">
+      <c r="J15" s="73">
         <f>I15-H15</f>
         <v>0.58019999999999994</v>
       </c>
@@ -9084,15 +9140,15 @@
       <c r="G16" s="4">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H16" s="110">
+      <c r="H16" s="72">
         <f t="shared" ref="H16:H20" si="7">C16*G16</f>
         <v>4.2768E-2</v>
       </c>
-      <c r="I16" s="111">
+      <c r="I16" s="73">
         <f>J15</f>
         <v>0.58019999999999994</v>
       </c>
-      <c r="J16" s="111">
+      <c r="J16" s="73">
         <f t="shared" ref="J16:J20" si="8">I16-H16</f>
         <v>0.53743199999999991</v>
       </c>
@@ -9124,15 +9180,15 @@
       <c r="G17" s="4">
         <v>2.7E-2</v>
       </c>
-      <c r="H17" s="110">
+      <c r="H17" s="72">
         <f t="shared" si="7"/>
         <v>3.8936700000000005E-2</v>
       </c>
-      <c r="I17" s="111">
+      <c r="I17" s="73">
         <f t="shared" ref="I17:I23" si="9">J16</f>
         <v>0.53743199999999991</v>
       </c>
-      <c r="J17" s="111">
+      <c r="J17" s="73">
         <f t="shared" si="8"/>
         <v>0.49849529999999992</v>
       </c>
@@ -9164,15 +9220,15 @@
       <c r="G18" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H18" s="110">
+      <c r="H18" s="72">
         <f t="shared" si="7"/>
         <v>5.8544200000000012E-2</v>
       </c>
-      <c r="I18" s="111">
+      <c r="I18" s="73">
         <f t="shared" si="9"/>
         <v>0.49849529999999992</v>
       </c>
-      <c r="J18" s="111">
+      <c r="J18" s="73">
         <f t="shared" si="8"/>
         <v>0.43995109999999993</v>
       </c>
@@ -9204,15 +9260,15 @@
       <c r="G19" s="4">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="H19" s="110">
+      <c r="H19" s="72">
         <f t="shared" si="7"/>
         <v>1.0769990000000002E-2</v>
       </c>
-      <c r="I19" s="111">
+      <c r="I19" s="73">
         <f t="shared" si="9"/>
         <v>0.43995109999999993</v>
       </c>
-      <c r="J19" s="111">
+      <c r="J19" s="73">
         <f t="shared" si="8"/>
         <v>0.42918110999999992</v>
       </c>
@@ -9244,15 +9300,15 @@
       <c r="G20" s="4">
         <v>4.86E-4</v>
       </c>
-      <c r="H20" s="110">
+      <c r="H20" s="72">
         <f t="shared" si="7"/>
         <v>7.5913200000000004E-4</v>
       </c>
-      <c r="I20" s="111">
+      <c r="I20" s="73">
         <f t="shared" si="9"/>
         <v>0.42918110999999992</v>
       </c>
-      <c r="J20" s="111">
+      <c r="J20" s="73">
         <f t="shared" si="8"/>
         <v>0.42842197799999993</v>
       </c>
@@ -9284,15 +9340,15 @@
       <c r="G21" s="4">
         <v>2.9399999999999999E-4</v>
       </c>
-      <c r="H21" s="110">
+      <c r="H21" s="72">
         <f t="shared" ref="H21:H23" si="10">C21*G21</f>
         <v>3.9584160000000001E-4</v>
       </c>
-      <c r="I21" s="111">
+      <c r="I21" s="73">
         <f t="shared" si="9"/>
         <v>0.42842197799999993</v>
       </c>
-      <c r="J21" s="111">
+      <c r="J21" s="73">
         <f t="shared" ref="J21:J23" si="11">I21-H21</f>
         <v>0.42802613639999992</v>
       </c>
@@ -9324,15 +9380,15 @@
       <c r="G22" s="4">
         <v>1.18E-4</v>
       </c>
-      <c r="H22" s="110">
+      <c r="H22" s="72">
         <f t="shared" si="10"/>
         <v>8.7225600000000007E-5</v>
       </c>
-      <c r="I22" s="111">
+      <c r="I22" s="73">
         <f t="shared" si="9"/>
         <v>0.42802613639999992</v>
       </c>
-      <c r="J22" s="111">
+      <c r="J22" s="73">
         <f t="shared" si="11"/>
         <v>0.42793891079999991</v>
       </c>
@@ -9364,15 +9420,15 @@
       <c r="G23" s="4">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H23" s="110">
+      <c r="H23" s="72">
         <f t="shared" si="10"/>
         <v>1.3648799999999997E-2</v>
       </c>
-      <c r="I23" s="111">
+      <c r="I23" s="73">
         <f t="shared" si="9"/>
         <v>0.42793891079999991</v>
       </c>
-      <c r="J23" s="111">
+      <c r="J23" s="73">
         <f t="shared" si="11"/>
         <v>0.41429011079999989</v>
       </c>
@@ -9382,32 +9438,32 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="81"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="84"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="84"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -9432,14 +9488,14 @@
       <c r="G26" s="4">
         <v>5.2600000000000001E-2</v>
       </c>
-      <c r="H26" s="110">
+      <c r="H26" s="72">
         <f>C26*G26</f>
         <v>2.8930000000000004E-2</v>
       </c>
-      <c r="I26" s="111">
+      <c r="I26" s="73">
         <v>0.6</v>
       </c>
-      <c r="J26" s="111">
+      <c r="J26" s="73">
         <f>I26-H26</f>
         <v>0.57106999999999997</v>
       </c>
@@ -9471,15 +9527,15 @@
       <c r="G27" s="4">
         <v>1.67E-2</v>
       </c>
-      <c r="H27" s="110">
+      <c r="H27" s="72">
         <f t="shared" ref="H27:H30" si="13">C27*G27</f>
         <v>1.9839600000000002E-2</v>
       </c>
-      <c r="I27" s="111">
+      <c r="I27" s="73">
         <f>J26</f>
         <v>0.57106999999999997</v>
       </c>
-      <c r="J27" s="111">
+      <c r="J27" s="73">
         <f t="shared" ref="J27:J30" si="14">I27-H27</f>
         <v>0.55123040000000001</v>
       </c>
@@ -9511,15 +9567,15 @@
       <c r="G28" s="4">
         <v>0.02</v>
       </c>
-      <c r="H28" s="110">
+      <c r="H28" s="72">
         <f t="shared" si="13"/>
         <v>2.8842000000000003E-2</v>
       </c>
-      <c r="I28" s="111">
+      <c r="I28" s="73">
         <f t="shared" ref="I28:I30" si="15">J27</f>
         <v>0.55123040000000001</v>
       </c>
-      <c r="J28" s="111">
+      <c r="J28" s="73">
         <f t="shared" si="14"/>
         <v>0.52238839999999997</v>
       </c>
@@ -9551,15 +9607,15 @@
       <c r="G29" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H29" s="110">
+      <c r="H29" s="72">
         <f t="shared" si="13"/>
         <v>2.9272100000000006E-2</v>
       </c>
-      <c r="I29" s="111">
+      <c r="I29" s="73">
         <f t="shared" si="15"/>
         <v>0.52238839999999997</v>
       </c>
-      <c r="J29" s="111">
+      <c r="J29" s="73">
         <f t="shared" si="14"/>
         <v>0.49311629999999995</v>
       </c>
@@ -9591,15 +9647,15 @@
       <c r="G30" s="4">
         <v>2.7E-2</v>
       </c>
-      <c r="H30" s="110">
+      <c r="H30" s="72">
         <f t="shared" si="13"/>
         <v>2.3462999999999999E-3</v>
       </c>
-      <c r="I30" s="111">
+      <c r="I30" s="73">
         <f t="shared" si="15"/>
         <v>0.49311629999999995</v>
       </c>
-      <c r="J30" s="111">
+      <c r="J30" s="73">
         <f t="shared" si="14"/>
         <v>0.49076999999999993</v>
       </c>
@@ -9609,32 +9665,32 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="80"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="81"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="84"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="81"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="84"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -9659,14 +9715,14 @@
       <c r="G33" s="4">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H33" s="110">
+      <c r="H33" s="72">
         <f>C33*G33</f>
         <v>2.9150000000000002E-2</v>
       </c>
-      <c r="I33" s="111">
+      <c r="I33" s="73">
         <v>0.6</v>
       </c>
-      <c r="J33" s="111">
+      <c r="J33" s="73">
         <f>I33-H33</f>
         <v>0.57084999999999997</v>
       </c>
@@ -9698,15 +9754,15 @@
       <c r="G34" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H34" s="110">
+      <c r="H34" s="72">
         <f t="shared" ref="H34:H38" si="17">C34*G34</f>
         <v>1.35993E-2</v>
       </c>
-      <c r="I34" s="111">
+      <c r="I34" s="73">
         <f>J33</f>
         <v>0.57084999999999997</v>
       </c>
-      <c r="J34" s="111">
+      <c r="J34" s="73">
         <f t="shared" ref="J34:J38" si="18">I34-H34</f>
         <v>0.55725069999999999</v>
       </c>
@@ -9738,15 +9794,15 @@
       <c r="G35" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="H35" s="110">
+      <c r="H35" s="72">
         <f t="shared" si="17"/>
         <v>8.8704000000000005E-3</v>
       </c>
-      <c r="I35" s="111">
+      <c r="I35" s="73">
         <f t="shared" ref="I35:I37" si="19">J34</f>
         <v>0.55725069999999999</v>
       </c>
-      <c r="J35" s="111">
+      <c r="J35" s="73">
         <f t="shared" si="18"/>
         <v>0.54838030000000004</v>
       </c>
@@ -9778,15 +9834,15 @@
       <c r="G36" s="4">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="H36" s="110">
+      <c r="H36" s="72">
         <f t="shared" si="17"/>
         <v>1.0097999999999999E-2</v>
       </c>
-      <c r="I36" s="111">
+      <c r="I36" s="73">
         <f t="shared" si="19"/>
         <v>0.54838030000000004</v>
       </c>
-      <c r="J36" s="111">
+      <c r="J36" s="73">
         <f t="shared" si="18"/>
         <v>0.53828229999999999</v>
       </c>
@@ -9818,15 +9874,15 @@
       <c r="G37" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H37" s="110">
+      <c r="H37" s="72">
         <f t="shared" ref="H37" si="20">C37*G37</f>
         <v>1.0934000000000001E-2</v>
       </c>
-      <c r="I37" s="111">
+      <c r="I37" s="73">
         <f t="shared" si="19"/>
         <v>0.53828229999999999</v>
       </c>
-      <c r="J37" s="111">
+      <c r="J37" s="73">
         <f t="shared" ref="J37" si="21">I37-H37</f>
         <v>0.52734829999999999</v>
       </c>
@@ -9858,15 +9914,15 @@
       <c r="G38" s="4">
         <v>0.06</v>
       </c>
-      <c r="H38" s="110">
+      <c r="H38" s="72">
         <f t="shared" si="17"/>
         <v>1.7754000000000002E-2</v>
       </c>
-      <c r="I38" s="111">
+      <c r="I38" s="73">
         <f>J36</f>
         <v>0.53828229999999999</v>
       </c>
-      <c r="J38" s="111">
+      <c r="J38" s="73">
         <f t="shared" si="18"/>
         <v>0.52052829999999994</v>
       </c>
@@ -9876,18 +9932,18 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="B39" s="80"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="81"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="84"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -9912,14 +9968,14 @@
       <c r="G40" s="4">
         <v>0.08</v>
       </c>
-      <c r="H40" s="110">
+      <c r="H40" s="72">
         <f>C40*G40</f>
         <v>9.0816000000000022E-2</v>
       </c>
-      <c r="I40" s="111">
+      <c r="I40" s="73">
         <v>0.6</v>
       </c>
-      <c r="J40" s="111">
+      <c r="J40" s="73">
         <f>I40-H40</f>
         <v>0.50918399999999997</v>
       </c>
@@ -9951,15 +10007,15 @@
       <c r="G41" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H41" s="110">
+      <c r="H41" s="72">
         <f t="shared" ref="H41:H45" si="23">C41*G41</f>
         <v>1.7138E-2</v>
       </c>
-      <c r="I41" s="111">
+      <c r="I41" s="73">
         <f>J40</f>
         <v>0.50918399999999997</v>
       </c>
-      <c r="J41" s="111">
+      <c r="J41" s="73">
         <f t="shared" ref="J41:J45" si="24">I41-H41</f>
         <v>0.49204599999999998</v>
       </c>
@@ -9991,15 +10047,15 @@
       <c r="G42" s="4">
         <v>2.7E-2</v>
       </c>
-      <c r="H42" s="110">
+      <c r="H42" s="72">
         <f t="shared" si="23"/>
         <v>2.3462999999999999E-3</v>
       </c>
-      <c r="I42" s="111">
+      <c r="I42" s="73">
         <f t="shared" ref="I42:I46" si="25">J41</f>
         <v>0.49204599999999998</v>
       </c>
-      <c r="J42" s="111">
+      <c r="J42" s="73">
         <f t="shared" si="24"/>
         <v>0.48969969999999996</v>
       </c>
@@ -10031,15 +10087,15 @@
       <c r="G43" s="4">
         <v>0.06</v>
       </c>
-      <c r="H43" s="110">
+      <c r="H43" s="72">
         <f t="shared" si="23"/>
         <v>1.7754000000000002E-2</v>
       </c>
-      <c r="I43" s="111">
+      <c r="I43" s="73">
         <f t="shared" si="25"/>
         <v>0.48969969999999996</v>
       </c>
-      <c r="J43" s="111">
+      <c r="J43" s="73">
         <f t="shared" si="24"/>
         <v>0.47194569999999997</v>
       </c>
@@ -10071,15 +10127,15 @@
       <c r="G44" s="4">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H44" s="110">
+      <c r="H44" s="72">
         <f t="shared" si="23"/>
         <v>5.9004000000000001E-3</v>
       </c>
-      <c r="I44" s="111">
+      <c r="I44" s="73">
         <f t="shared" si="25"/>
         <v>0.47194569999999997</v>
       </c>
-      <c r="J44" s="111">
+      <c r="J44" s="73">
         <f t="shared" si="24"/>
         <v>0.4660453</v>
       </c>
@@ -10111,15 +10167,15 @@
       <c r="G45" s="4">
         <v>0.05</v>
       </c>
-      <c r="H45" s="110">
+      <c r="H45" s="72">
         <f t="shared" si="23"/>
         <v>4.3450000000000008E-3</v>
       </c>
-      <c r="I45" s="111">
+      <c r="I45" s="73">
         <f t="shared" si="25"/>
         <v>0.4660453</v>
       </c>
-      <c r="J45" s="111">
+      <c r="J45" s="73">
         <f t="shared" si="24"/>
         <v>0.46170030000000001</v>
       </c>
@@ -10151,15 +10207,15 @@
       <c r="G46" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H46" s="110">
+      <c r="H46" s="72">
         <f t="shared" ref="H46" si="26">C46*G46</f>
         <v>2.3575199999999998E-2</v>
       </c>
-      <c r="I46" s="111">
+      <c r="I46" s="73">
         <f t="shared" si="25"/>
         <v>0.46170030000000001</v>
       </c>
-      <c r="J46" s="111">
+      <c r="J46" s="73">
         <f t="shared" ref="J46" si="27">I46-H46</f>
         <v>0.43812509999999999</v>
       </c>
@@ -10170,13 +10226,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A32:J32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A1:A2"/>
@@ -10185,6 +10234,13 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A32:J32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>